<commit_message>
Update the code for ICM
</commit_message>
<xml_diff>
--- a/output/df_icm.xlsx
+++ b/output/df_icm.xlsx
@@ -12,7 +12,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="146">
+  <si>
+    <t>PopID</t>
+  </si>
   <si>
     <t>Pop</t>
   </si>
@@ -33,6 +36,9 @@
   </si>
   <si>
     <t>bnft_hi</t>
+  </si>
+  <si>
+    <t>loss1</t>
   </si>
   <si>
     <t>loss2</t>
@@ -670,37 +676,43 @@
       <c r="BG1" t="s">
         <v>57</v>
       </c>
+      <c r="BH1" t="s">
+        <v>58</v>
+      </c>
+      <c r="BI1" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C2" t="n">
+        <v>60</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D2" t="n">
         <v>17.888403142397586</v>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>16.090950122217105</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>19.049125018924613</v>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>3.82522615345769</v>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
         <v>2.798151073695358</v>
       </c>
-      <c r="H2" t="n">
+      <c r="I2" t="n">
         <v>5.0848615630917715</v>
       </c>
-      <c r="I2" t="n">
-        <v>0.008193875844705722</v>
-      </c>
-      <c r="J2" t="n">
-        <v>0.008193875844705722</v>
+      <c r="J2" t="e">
+        <v>#N/A</v>
       </c>
       <c r="K2" t="n">
         <v>0.008193875844705722</v>
@@ -727,10 +739,10 @@
         <v>0.008193875844705722</v>
       </c>
       <c r="S2" t="n">
-        <v>0.00738576781838578</v>
+        <v>0.008193875844705722</v>
       </c>
       <c r="T2" t="n">
-        <v>0.00738576781838578</v>
+        <v>0.008193875844705722</v>
       </c>
       <c r="U2" t="n">
         <v>0.00738576781838578</v>
@@ -757,10 +769,10 @@
         <v>0.00738576781838578</v>
       </c>
       <c r="AC2" t="n">
-        <v>0.005037358173549755</v>
+        <v>0.00738576781838578</v>
       </c>
       <c r="AD2" t="n">
-        <v>0.005037358173549755</v>
+        <v>0.00738576781838578</v>
       </c>
       <c r="AE2" t="n">
         <v>0.005037358173549755</v>
@@ -787,10 +799,10 @@
         <v>0.005037358173549755</v>
       </c>
       <c r="AM2" t="n">
-        <v>0.004982890994598499</v>
+        <v>0.005037358173549755</v>
       </c>
       <c r="AN2" t="n">
-        <v>0.004982890994598499</v>
+        <v>0.005037358173549755</v>
       </c>
       <c r="AO2" t="n">
         <v>0.004982890994598499</v>
@@ -817,10 +829,10 @@
         <v>0.004982890994598499</v>
       </c>
       <c r="AW2" t="n">
-        <v>0.004939502369460946</v>
+        <v>0.004982890994598499</v>
       </c>
       <c r="AX2" t="n">
-        <v>0.004939502369460946</v>
+        <v>0.004982890994598499</v>
       </c>
       <c r="AY2" t="n">
         <v>0.004939502369460946</v>
@@ -847,39 +859,45 @@
         <v>0.004939502369460946</v>
       </c>
       <c r="BG2" t="n">
+        <v>0.004939502369460946</v>
+      </c>
+      <c r="BH2" t="n">
+        <v>0.004939502369460946</v>
+      </c>
+      <c r="BI2" t="n">
         <v>0.004939502369460946</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B3" t="s">
-        <v>102</v>
-      </c>
-      <c r="C3" t="n">
+        <v>61</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D3" t="n">
         <v>16.076780969327302</v>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
         <v>14.594196326113055</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>17.176875685356176</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>2.1259032697960762</v>
       </c>
-      <c r="G3" t="n">
+      <c r="H3" t="n">
         <v>0.9096430728335072</v>
       </c>
-      <c r="H3" t="n">
+      <c r="I3" t="n">
         <v>3.697689398113628</v>
       </c>
-      <c r="I3" t="n">
-        <v>0.006045282309819733</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0.006045282309819733</v>
+      <c r="J3" t="e">
+        <v>#N/A</v>
       </c>
       <c r="K3" t="n">
         <v>0.006045282309819733</v>
@@ -906,10 +924,10 @@
         <v>0.006045282309819733</v>
       </c>
       <c r="S3" t="n">
-        <v>0.0054327914602032125</v>
+        <v>0.006045282309819733</v>
       </c>
       <c r="T3" t="n">
-        <v>0.0054327914602032125</v>
+        <v>0.006045282309819733</v>
       </c>
       <c r="U3" t="n">
         <v>0.0054327914602032125</v>
@@ -936,10 +954,10 @@
         <v>0.0054327914602032125</v>
       </c>
       <c r="AC3" t="n">
-        <v>0.0027770100110659614</v>
+        <v>0.0054327914602032125</v>
       </c>
       <c r="AD3" t="n">
-        <v>0.0027770100110659614</v>
+        <v>0.0054327914602032125</v>
       </c>
       <c r="AE3" t="n">
         <v>0.0027770100110659614</v>
@@ -966,10 +984,10 @@
         <v>0.0027770100110659614</v>
       </c>
       <c r="AM3" t="n">
-        <v>0.0027328132690787044</v>
+        <v>0.0027770100110659614</v>
       </c>
       <c r="AN3" t="n">
-        <v>0.0027328132690787044</v>
+        <v>0.0027770100110659614</v>
       </c>
       <c r="AO3" t="n">
         <v>0.0027328132690787044</v>
@@ -996,10 +1014,10 @@
         <v>0.0027328132690787044</v>
       </c>
       <c r="AW3" t="n">
-        <v>0.0027065931463456927</v>
+        <v>0.0027328132690787044</v>
       </c>
       <c r="AX3" t="n">
-        <v>0.0027065931463456927</v>
+        <v>0.0027328132690787044</v>
       </c>
       <c r="AY3" t="n">
         <v>0.0027065931463456927</v>
@@ -1026,39 +1044,45 @@
         <v>0.0027065931463456927</v>
       </c>
       <c r="BG3" t="n">
+        <v>0.0027065931463456927</v>
+      </c>
+      <c r="BH3" t="n">
+        <v>0.0027065931463456927</v>
+      </c>
+      <c r="BI3" t="n">
         <v>0.0027065931463456927</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C4" t="n">
+        <v>62</v>
+      </c>
+      <c r="B4" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D4" t="n">
         <v>15.581455459604527</v>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
         <v>14.21504115513983</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>16.628385694748957</v>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
         <v>10.337087671890476</v>
       </c>
-      <c r="G4" t="n">
+      <c r="H4" t="n">
         <v>8.65449158825991</v>
       </c>
-      <c r="H4" t="n">
+      <c r="I4" t="n">
         <v>11.924108007262202</v>
       </c>
-      <c r="I4" t="n">
-        <v>0.02067675632171424</v>
-      </c>
-      <c r="J4" t="n">
-        <v>0.02067675632171424</v>
+      <c r="J4" t="e">
+        <v>#N/A</v>
       </c>
       <c r="K4" t="n">
         <v>0.02067675632171424</v>
@@ -1085,10 +1109,10 @@
         <v>0.02067675632171424</v>
       </c>
       <c r="S4" t="n">
-        <v>0.020298504643344817</v>
+        <v>0.02067675632171424</v>
       </c>
       <c r="T4" t="n">
-        <v>0.020298504643344817</v>
+        <v>0.02067675632171424</v>
       </c>
       <c r="U4" t="n">
         <v>0.020298504643344817</v>
@@ -1115,10 +1139,10 @@
         <v>0.020298504643344817</v>
       </c>
       <c r="AC4" t="n">
-        <v>0.019926854699489294</v>
+        <v>0.020298504643344817</v>
       </c>
       <c r="AD4" t="n">
-        <v>0.019926854699489294</v>
+        <v>0.020298504643344817</v>
       </c>
       <c r="AE4" t="n">
         <v>0.019926854699489294</v>
@@ -1145,10 +1169,10 @@
         <v>0.019926854699489294</v>
       </c>
       <c r="AM4" t="n">
-        <v>0.01957858486993187</v>
+        <v>0.019926854699489294</v>
       </c>
       <c r="AN4" t="n">
-        <v>0.01957858486993187</v>
+        <v>0.019926854699489294</v>
       </c>
       <c r="AO4" t="n">
         <v>0.01957858486993187</v>
@@ -1175,10 +1199,10 @@
         <v>0.01957858486993187</v>
       </c>
       <c r="AW4" t="n">
-        <v>0.019240790922439643</v>
+        <v>0.01957858486993187</v>
       </c>
       <c r="AX4" t="n">
-        <v>0.019240790922439643</v>
+        <v>0.01957858486993187</v>
       </c>
       <c r="AY4" t="n">
         <v>0.019240790922439643</v>
@@ -1205,39 +1229,45 @@
         <v>0.019240790922439643</v>
       </c>
       <c r="BG4" t="n">
+        <v>0.019240790922439643</v>
+      </c>
+      <c r="BH4" t="n">
+        <v>0.019240790922439643</v>
+      </c>
+      <c r="BI4" t="n">
         <v>0.019240790922439643</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B5" t="s">
-        <v>104</v>
-      </c>
-      <c r="C5" t="n">
+        <v>63</v>
+      </c>
+      <c r="B5" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D5" t="n">
         <v>5.668119835101866</v>
       </c>
-      <c r="D5" t="n">
+      <c r="E5" t="n">
         <v>4.6872113369591775</v>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
         <v>7.535647046213431</v>
       </c>
-      <c r="F5" t="n">
+      <c r="G5" t="n">
         <v>1.2031059881187165</v>
       </c>
-      <c r="G5" t="n">
+      <c r="H5" t="n">
         <v>0.9627248741624495</v>
       </c>
-      <c r="H5" t="n">
+      <c r="I5" t="n">
         <v>1.5428189040287976</v>
       </c>
-      <c r="I5" t="n">
-        <v>0.01115370328520946</v>
-      </c>
-      <c r="J5" t="n">
-        <v>0.01115370328520946</v>
+      <c r="J5" t="e">
+        <v>#N/A</v>
       </c>
       <c r="K5" t="n">
         <v>0.01115370328520946</v>
@@ -1264,10 +1294,10 @@
         <v>0.01115370328520946</v>
       </c>
       <c r="S5" t="n">
-        <v>0.010618568555493146</v>
+        <v>0.01115370328520946</v>
       </c>
       <c r="T5" t="n">
-        <v>0.010618568555493146</v>
+        <v>0.01115370328520946</v>
       </c>
       <c r="U5" t="n">
         <v>0.010618568555493146</v>
@@ -1294,10 +1324,10 @@
         <v>0.010618568555493146</v>
       </c>
       <c r="AC5" t="n">
-        <v>0.010088038012143086</v>
+        <v>0.010618568555493146</v>
       </c>
       <c r="AD5" t="n">
-        <v>0.010088038012143086</v>
+        <v>0.010618568555493146</v>
       </c>
       <c r="AE5" t="n">
         <v>0.010088038012143086</v>
@@ -1324,10 +1354,10 @@
         <v>0.010088038012143086</v>
       </c>
       <c r="AM5" t="n">
-        <v>0.007749245201818545</v>
+        <v>0.010088038012143086</v>
       </c>
       <c r="AN5" t="n">
-        <v>0.007749245201818545</v>
+        <v>0.010088038012143086</v>
       </c>
       <c r="AO5" t="n">
         <v>0.007749245201818545</v>
@@ -1354,10 +1384,10 @@
         <v>0.007749245201818545</v>
       </c>
       <c r="AW5" t="n">
-        <v>0.0034653921030063373</v>
+        <v>0.007749245201818545</v>
       </c>
       <c r="AX5" t="n">
-        <v>0.0034653921030063373</v>
+        <v>0.007749245201818545</v>
       </c>
       <c r="AY5" t="n">
         <v>0.0034653921030063373</v>
@@ -1384,39 +1414,45 @@
         <v>0.0034653921030063373</v>
       </c>
       <c r="BG5" t="n">
+        <v>0.0034653921030063373</v>
+      </c>
+      <c r="BH5" t="n">
+        <v>0.0034653921030063373</v>
+      </c>
+      <c r="BI5" t="n">
         <v>0.0034653921030063373</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>62</v>
-      </c>
-      <c r="B6" t="s">
-        <v>105</v>
-      </c>
-      <c r="C6" t="n">
+        <v>64</v>
+      </c>
+      <c r="B6" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>107</v>
+      </c>
+      <c r="D6" t="n">
         <v>2.4253962345695737</v>
       </c>
-      <c r="D6" t="n">
+      <c r="E6" t="n">
         <v>1.8117004481697832</v>
       </c>
-      <c r="E6" t="n">
+      <c r="F6" t="n">
         <v>3.486428489811849</v>
       </c>
-      <c r="F6" t="n">
+      <c r="G6" t="n">
         <v>1.327121028577928</v>
       </c>
-      <c r="G6" t="n">
+      <c r="H6" t="n">
         <v>1.0881306472518255</v>
       </c>
-      <c r="H6" t="n">
+      <c r="I6" t="n">
         <v>1.7584516569371966</v>
       </c>
-      <c r="I6" t="n">
-        <v>0.02512875582972742</v>
-      </c>
-      <c r="J6" t="n">
-        <v>0.02512875582972742</v>
+      <c r="J6" t="e">
+        <v>#N/A</v>
       </c>
       <c r="K6" t="n">
         <v>0.02512875582972742</v>
@@ -1443,10 +1479,10 @@
         <v>0.02512875582972742</v>
       </c>
       <c r="S6" t="n">
-        <v>0.02142915427308718</v>
+        <v>0.02512875582972742</v>
       </c>
       <c r="T6" t="n">
-        <v>0.02142915427308718</v>
+        <v>0.02512875582972742</v>
       </c>
       <c r="U6" t="n">
         <v>0.02142915427308718</v>
@@ -1473,10 +1509,10 @@
         <v>0.02142915427308718</v>
       </c>
       <c r="AC6" t="n">
-        <v>0.01823702477580442</v>
+        <v>0.02142915427308718</v>
       </c>
       <c r="AD6" t="n">
-        <v>0.01823702477580442</v>
+        <v>0.02142915427308718</v>
       </c>
       <c r="AE6" t="n">
         <v>0.01823702477580442</v>
@@ -1503,10 +1539,10 @@
         <v>0.01823702477580442</v>
       </c>
       <c r="AM6" t="n">
-        <v>0.015004516950583746</v>
+        <v>0.01823702477580442</v>
       </c>
       <c r="AN6" t="n">
-        <v>0.015004516950583746</v>
+        <v>0.01823702477580442</v>
       </c>
       <c r="AO6" t="n">
         <v>0.015004516950583746</v>
@@ -1533,10 +1569,10 @@
         <v>0.015004516950583746</v>
       </c>
       <c r="AW6" t="n">
-        <v>0.011017954755425292</v>
+        <v>0.015004516950583746</v>
       </c>
       <c r="AX6" t="n">
-        <v>0.011017954755425292</v>
+        <v>0.015004516950583746</v>
       </c>
       <c r="AY6" t="n">
         <v>0.011017954755425292</v>
@@ -1563,39 +1599,45 @@
         <v>0.011017954755425292</v>
       </c>
       <c r="BG6" t="n">
+        <v>0.011017954755425292</v>
+      </c>
+      <c r="BH6" t="n">
+        <v>0.011017954755425292</v>
+      </c>
+      <c r="BI6" t="n">
         <v>0.011017954755425292</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>63</v>
-      </c>
-      <c r="B7" t="s">
-        <v>106</v>
-      </c>
-      <c r="C7" t="n">
+        <v>65</v>
+      </c>
+      <c r="B7" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>108</v>
+      </c>
+      <c r="D7" t="n">
         <v>4.257316560900319</v>
       </c>
-      <c r="D7" t="n">
+      <c r="E7" t="n">
         <v>4.1420421827610205</v>
       </c>
-      <c r="E7" t="n">
+      <c r="F7" t="n">
         <v>4.356557093967558</v>
       </c>
-      <c r="F7" t="n">
+      <c r="G7" t="n">
         <v>1.0778471708260804</v>
       </c>
-      <c r="G7" t="n">
+      <c r="H7" t="n">
         <v>0.8134687395374914</v>
       </c>
-      <c r="H7" t="n">
+      <c r="I7" t="n">
         <v>1.328395100843189</v>
       </c>
-      <c r="I7" t="n">
-        <v>0.015395529372058148</v>
-      </c>
-      <c r="J7" t="n">
-        <v>0.015395529372058148</v>
+      <c r="J7" t="e">
+        <v>#N/A</v>
       </c>
       <c r="K7" t="n">
         <v>0.015395529372058148</v>
@@ -1622,10 +1664,10 @@
         <v>0.015395529372058148</v>
       </c>
       <c r="S7" t="n">
-        <v>0.007533640927280416</v>
+        <v>0.015395529372058148</v>
       </c>
       <c r="T7" t="n">
-        <v>0.007533640927280416</v>
+        <v>0.015395529372058148</v>
       </c>
       <c r="U7" t="n">
         <v>0.007533640927280416</v>
@@ -1652,10 +1694,10 @@
         <v>0.007533640927280416</v>
       </c>
       <c r="AC7" t="n">
-        <v>0.004733357918274938</v>
+        <v>0.007533640927280416</v>
       </c>
       <c r="AD7" t="n">
-        <v>0.004733357918274938</v>
+        <v>0.007533640927280416</v>
       </c>
       <c r="AE7" t="n">
         <v>0.004733357918274938</v>
@@ -1682,10 +1724,10 @@
         <v>0.004733357918274938</v>
       </c>
       <c r="AM7" t="n">
-        <v>0.004472972129041297</v>
+        <v>0.004733357918274938</v>
       </c>
       <c r="AN7" t="n">
-        <v>0.004472972129041297</v>
+        <v>0.004733357918274938</v>
       </c>
       <c r="AO7" t="n">
         <v>0.004472972129041297</v>
@@ -1712,10 +1754,10 @@
         <v>0.004472972129041297</v>
       </c>
       <c r="AW7" t="n">
-        <v>0.0042269128208183735</v>
+        <v>0.004472972129041297</v>
       </c>
       <c r="AX7" t="n">
-        <v>0.0042269128208183735</v>
+        <v>0.004472972129041297</v>
       </c>
       <c r="AY7" t="n">
         <v>0.0042269128208183735</v>
@@ -1742,39 +1784,45 @@
         <v>0.0042269128208183735</v>
       </c>
       <c r="BG7" t="n">
+        <v>0.0042269128208183735</v>
+      </c>
+      <c r="BH7" t="n">
+        <v>0.0042269128208183735</v>
+      </c>
+      <c r="BI7" t="n">
         <v>0.0042269128208183735</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>64</v>
-      </c>
-      <c r="B8" t="s">
-        <v>107</v>
-      </c>
-      <c r="C8" t="n">
+        <v>66</v>
+      </c>
+      <c r="B8" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D8" t="n">
         <v>2.0757393667439024</v>
       </c>
-      <c r="D8" t="n">
+      <c r="E8" t="n">
         <v>1.56209785567012</v>
       </c>
-      <c r="E8" t="n">
+      <c r="F8" t="n">
         <v>2.5562759689902057</v>
       </c>
-      <c r="F8" t="n">
+      <c r="G8" t="n">
         <v>0.7775417310807191</v>
       </c>
-      <c r="G8" t="n">
+      <c r="H8" t="n">
         <v>0.5664305637279399</v>
       </c>
-      <c r="H8" t="n">
+      <c r="I8" t="n">
         <v>1.072688679619742</v>
       </c>
-      <c r="I8" t="n">
-        <v>0.02394627327520079</v>
-      </c>
-      <c r="J8" t="n">
-        <v>0.02394627327520079</v>
+      <c r="J8" t="e">
+        <v>#N/A</v>
       </c>
       <c r="K8" t="n">
         <v>0.02394627327520079</v>
@@ -1801,10 +1849,10 @@
         <v>0.02394627327520079</v>
       </c>
       <c r="S8" t="n">
-        <v>0.018480392465602104</v>
+        <v>0.02394627327520079</v>
       </c>
       <c r="T8" t="n">
-        <v>0.018480392465602104</v>
+        <v>0.02394627327520079</v>
       </c>
       <c r="U8" t="n">
         <v>0.018480392465602104</v>
@@ -1831,10 +1879,10 @@
         <v>0.018480392465602104</v>
       </c>
       <c r="AC8" t="n">
-        <v>0.01114577661737054</v>
+        <v>0.018480392465602104</v>
       </c>
       <c r="AD8" t="n">
-        <v>0.01114577661737054</v>
+        <v>0.018480392465602104</v>
       </c>
       <c r="AE8" t="n">
         <v>0.01114577661737054</v>
@@ -1861,10 +1909,10 @@
         <v>0.01114577661737054</v>
       </c>
       <c r="AM8" t="n">
-        <v>0.0043098451994603385</v>
+        <v>0.01114577661737054</v>
       </c>
       <c r="AN8" t="n">
-        <v>0.0043098451994603385</v>
+        <v>0.01114577661737054</v>
       </c>
       <c r="AO8" t="n">
         <v>0.0043098451994603385</v>
@@ -1891,10 +1939,10 @@
         <v>0.0043098451994603385</v>
       </c>
       <c r="AW8" t="n">
-        <v>0.00306340585234659</v>
+        <v>0.0043098451994603385</v>
       </c>
       <c r="AX8" t="n">
-        <v>0.00306340585234659</v>
+        <v>0.0043098451994603385</v>
       </c>
       <c r="AY8" t="n">
         <v>0.00306340585234659</v>
@@ -1921,39 +1969,45 @@
         <v>0.00306340585234659</v>
       </c>
       <c r="BG8" t="n">
+        <v>0.00306340585234659</v>
+      </c>
+      <c r="BH8" t="n">
+        <v>0.00306340585234659</v>
+      </c>
+      <c r="BI8" t="n">
         <v>0.00306340585234659</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>65</v>
-      </c>
-      <c r="B9" t="s">
-        <v>108</v>
-      </c>
-      <c r="C9" t="n">
+        <v>67</v>
+      </c>
+      <c r="B9" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>110</v>
+      </c>
+      <c r="D9" t="n">
         <v>4.671615613805379</v>
       </c>
-      <c r="D9" t="n">
+      <c r="E9" t="n">
         <v>3.8915885387009848</v>
       </c>
-      <c r="E9" t="n">
+      <c r="F9" t="n">
         <v>5.387089432549146</v>
       </c>
-      <c r="F9" t="n">
+      <c r="G9" t="n">
         <v>2.3070211791374415</v>
       </c>
-      <c r="G9" t="n">
+      <c r="H9" t="n">
         <v>1.720937790082615</v>
       </c>
-      <c r="H9" t="n">
+      <c r="I9" t="n">
         <v>3.0045473696094263</v>
       </c>
-      <c r="I9" t="n">
-        <v>0.025547898041614125</v>
-      </c>
-      <c r="J9" t="n">
-        <v>0.025547898041614125</v>
+      <c r="J9" t="e">
+        <v>#N/A</v>
       </c>
       <c r="K9" t="n">
         <v>0.025547898041614125</v>
@@ -1980,10 +2034,10 @@
         <v>0.025547898041614125</v>
       </c>
       <c r="S9" t="n">
-        <v>0.023228967464755314</v>
+        <v>0.025547898041614125</v>
       </c>
       <c r="T9" t="n">
-        <v>0.023228967464755314</v>
+        <v>0.025547898041614125</v>
       </c>
       <c r="U9" t="n">
         <v>0.023228967464755314</v>
@@ -2010,10 +2064,10 @@
         <v>0.023228967464755314</v>
       </c>
       <c r="AC9" t="n">
-        <v>0.021099819637660146</v>
+        <v>0.023228967464755314</v>
       </c>
       <c r="AD9" t="n">
-        <v>0.021099819637660146</v>
+        <v>0.023228967464755314</v>
       </c>
       <c r="AE9" t="n">
         <v>0.021099819637660146</v>
@@ -2040,10 +2094,10 @@
         <v>0.021099819637660146</v>
       </c>
       <c r="AM9" t="n">
-        <v>0.019162846426547954</v>
+        <v>0.021099819637660146</v>
       </c>
       <c r="AN9" t="n">
-        <v>0.019162846426547954</v>
+        <v>0.021099819637660146</v>
       </c>
       <c r="AO9" t="n">
         <v>0.019162846426547954</v>
@@ -2070,10 +2124,10 @@
         <v>0.019162846426547954</v>
       </c>
       <c r="AW9" t="n">
-        <v>0.017428650245688425</v>
+        <v>0.019162846426547954</v>
       </c>
       <c r="AX9" t="n">
-        <v>0.017428650245688425</v>
+        <v>0.019162846426547954</v>
       </c>
       <c r="AY9" t="n">
         <v>0.017428650245688425</v>
@@ -2100,39 +2154,45 @@
         <v>0.017428650245688425</v>
       </c>
       <c r="BG9" t="n">
+        <v>0.017428650245688425</v>
+      </c>
+      <c r="BH9" t="n">
+        <v>0.017428650245688425</v>
+      </c>
+      <c r="BI9" t="n">
         <v>0.017428650245688425</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>66</v>
-      </c>
-      <c r="B10" t="s">
-        <v>109</v>
-      </c>
-      <c r="C10" t="n">
+        <v>68</v>
+      </c>
+      <c r="B10" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>111</v>
+      </c>
+      <c r="D10" t="n">
         <v>10.052325816462625</v>
       </c>
-      <c r="D10" t="n">
+      <c r="E10" t="n">
         <v>9.146649671440315</v>
       </c>
-      <c r="E10" t="n">
+      <c r="F10" t="n">
         <v>10.959907765755737</v>
       </c>
-      <c r="F10" t="n">
+      <c r="G10" t="n">
         <v>7.314989756251974</v>
       </c>
-      <c r="G10" t="n">
+      <c r="H10" t="n">
         <v>6.761007488970354</v>
       </c>
-      <c r="H10" t="n">
+      <c r="I10" t="n">
         <v>8.066871409869975</v>
       </c>
-      <c r="I10" t="n">
-        <v>0.01861337127140379</v>
-      </c>
-      <c r="J10" t="n">
-        <v>0.01861337127140379</v>
+      <c r="J10" t="e">
+        <v>#N/A</v>
       </c>
       <c r="K10" t="n">
         <v>0.01861337127140379</v>
@@ -2159,10 +2219,10 @@
         <v>0.01861337127140379</v>
       </c>
       <c r="S10" t="n">
-        <v>0.01816219782134647</v>
+        <v>0.01861337127140379</v>
       </c>
       <c r="T10" t="n">
-        <v>0.01816219782134647</v>
+        <v>0.01861337127140379</v>
       </c>
       <c r="U10" t="n">
         <v>0.01816219782134647</v>
@@ -2189,10 +2249,10 @@
         <v>0.01816219782134647</v>
       </c>
       <c r="AC10" t="n">
-        <v>0.017726578078635848</v>
+        <v>0.01816219782134647</v>
       </c>
       <c r="AD10" t="n">
-        <v>0.017726578078635848</v>
+        <v>0.01816219782134647</v>
       </c>
       <c r="AE10" t="n">
         <v>0.017726578078635848</v>
@@ -2219,10 +2279,10 @@
         <v>0.017726578078635848</v>
       </c>
       <c r="AM10" t="n">
-        <v>0.01730797065642662</v>
+        <v>0.017726578078635848</v>
       </c>
       <c r="AN10" t="n">
-        <v>0.01730797065642662</v>
+        <v>0.017726578078635848</v>
       </c>
       <c r="AO10" t="n">
         <v>0.01730797065642662</v>
@@ -2249,10 +2309,10 @@
         <v>0.01730797065642662</v>
       </c>
       <c r="AW10" t="n">
-        <v>0.0168989962090051</v>
+        <v>0.01730797065642662</v>
       </c>
       <c r="AX10" t="n">
-        <v>0.0168989962090051</v>
+        <v>0.01730797065642662</v>
       </c>
       <c r="AY10" t="n">
         <v>0.0168989962090051</v>
@@ -2279,39 +2339,45 @@
         <v>0.0168989962090051</v>
       </c>
       <c r="BG10" t="n">
+        <v>0.0168989962090051</v>
+      </c>
+      <c r="BH10" t="n">
+        <v>0.0168989962090051</v>
+      </c>
+      <c r="BI10" t="n">
         <v>0.0168989962090051</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>67</v>
-      </c>
-      <c r="B11" t="s">
-        <v>110</v>
-      </c>
-      <c r="C11" t="n">
+        <v>69</v>
+      </c>
+      <c r="B11" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>112</v>
+      </c>
+      <c r="D11" t="n">
         <v>1.482740952892821</v>
       </c>
-      <c r="D11" t="n">
+      <c r="E11" t="n">
         <v>1.411605362718557</v>
       </c>
-      <c r="E11" t="n">
+      <c r="F11" t="n">
         <v>1.5521189341480355</v>
       </c>
-      <c r="F11" t="n">
+      <c r="G11" t="n">
         <v>0.5454519967899203</v>
       </c>
-      <c r="G11" t="n">
+      <c r="H11" t="n">
         <v>0.48033524029954155</v>
       </c>
-      <c r="H11" t="n">
+      <c r="I11" t="n">
         <v>0.6060589748518483</v>
       </c>
-      <c r="I11" t="n">
-        <v>0.007682391043536041</v>
-      </c>
-      <c r="J11" t="n">
-        <v>0.007682391043536041</v>
+      <c r="J11" t="e">
+        <v>#N/A</v>
       </c>
       <c r="K11" t="n">
         <v>0.007682391043536041</v>
@@ -2338,10 +2404,10 @@
         <v>0.007682391043536041</v>
       </c>
       <c r="S11" t="n">
-        <v>0.006598365025088093</v>
+        <v>0.007682391043536041</v>
       </c>
       <c r="T11" t="n">
-        <v>0.006598365025088093</v>
+        <v>0.007682391043536041</v>
       </c>
       <c r="U11" t="n">
         <v>0.006598365025088093</v>
@@ -2368,10 +2434,10 @@
         <v>0.006598365025088093</v>
       </c>
       <c r="AC11" t="n">
-        <v>0.005665720848355327</v>
+        <v>0.006598365025088093</v>
       </c>
       <c r="AD11" t="n">
-        <v>0.005665720848355327</v>
+        <v>0.006598365025088093</v>
       </c>
       <c r="AE11" t="n">
         <v>0.005665720848355327</v>
@@ -2398,10 +2464,10 @@
         <v>0.005665720848355327</v>
       </c>
       <c r="AM11" t="n">
-        <v>0.004871890710655235</v>
+        <v>0.005665720848355327</v>
       </c>
       <c r="AN11" t="n">
-        <v>0.004871890710655235</v>
+        <v>0.005665720848355327</v>
       </c>
       <c r="AO11" t="n">
         <v>0.004871890710655235</v>
@@ -2428,10 +2494,10 @@
         <v>0.004871890710655235</v>
       </c>
       <c r="AW11" t="n">
-        <v>0.004186715534897178</v>
+        <v>0.004871890710655235</v>
       </c>
       <c r="AX11" t="n">
-        <v>0.004186715534897178</v>
+        <v>0.004871890710655235</v>
       </c>
       <c r="AY11" t="n">
         <v>0.004186715534897178</v>
@@ -2458,39 +2524,45 @@
         <v>0.004186715534897178</v>
       </c>
       <c r="BG11" t="n">
+        <v>0.004186715534897178</v>
+      </c>
+      <c r="BH11" t="n">
+        <v>0.004186715534897178</v>
+      </c>
+      <c r="BI11" t="n">
         <v>0.004186715534897178</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>68</v>
-      </c>
-      <c r="B12" t="s">
-        <v>111</v>
-      </c>
-      <c r="C12" t="n">
+        <v>70</v>
+      </c>
+      <c r="B12" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>113</v>
+      </c>
+      <c r="D12" t="n">
         <v>7.807912026527482</v>
       </c>
-      <c r="D12" t="n">
+      <c r="E12" t="n">
         <v>7.144107564448529</v>
       </c>
-      <c r="E12" t="n">
+      <c r="F12" t="n">
         <v>8.306842165641113</v>
       </c>
-      <c r="F12" t="n">
+      <c r="G12" t="n">
         <v>2.1580517200908713</v>
       </c>
-      <c r="G12" t="n">
+      <c r="H12" t="n">
         <v>1.5344823450153864</v>
       </c>
-      <c r="H12" t="n">
+      <c r="I12" t="n">
         <v>2.6608842952338803</v>
       </c>
-      <c r="I12" t="n">
-        <v>0.005012590484129209</v>
-      </c>
-      <c r="J12" t="n">
-        <v>0.005012590484129209</v>
+      <c r="J12" t="e">
+        <v>#N/A</v>
       </c>
       <c r="K12" t="n">
         <v>0.005012590484129209</v>
@@ -2517,10 +2589,10 @@
         <v>0.005012590484129209</v>
       </c>
       <c r="S12" t="n">
-        <v>0.004899076395599699</v>
+        <v>0.005012590484129209</v>
       </c>
       <c r="T12" t="n">
-        <v>0.004899076395599699</v>
+        <v>0.005012590484129209</v>
       </c>
       <c r="U12" t="n">
         <v>0.004899076395599699</v>
@@ -2547,10 +2619,10 @@
         <v>0.004899076395599699</v>
       </c>
       <c r="AC12" t="n">
-        <v>0.004786431222115884</v>
+        <v>0.004899076395599699</v>
       </c>
       <c r="AD12" t="n">
-        <v>0.004786431222115884</v>
+        <v>0.004899076395599699</v>
       </c>
       <c r="AE12" t="n">
         <v>0.004786431222115884</v>
@@ -2577,10 +2649,10 @@
         <v>0.004786431222115884</v>
       </c>
       <c r="AM12" t="n">
-        <v>0.004676331886565688</v>
+        <v>0.004786431222115884</v>
       </c>
       <c r="AN12" t="n">
-        <v>0.004676331886565688</v>
+        <v>0.004786431222115884</v>
       </c>
       <c r="AO12" t="n">
         <v>0.004676331886565688</v>
@@ -2607,10 +2679,10 @@
         <v>0.004676331886565688</v>
       </c>
       <c r="AW12" t="n">
-        <v>0.0045687223044934555</v>
+        <v>0.004676331886565688</v>
       </c>
       <c r="AX12" t="n">
-        <v>0.0045687223044934555</v>
+        <v>0.004676331886565688</v>
       </c>
       <c r="AY12" t="n">
         <v>0.0045687223044934555</v>
@@ -2637,39 +2709,45 @@
         <v>0.0045687223044934555</v>
       </c>
       <c r="BG12" t="n">
+        <v>0.0045687223044934555</v>
+      </c>
+      <c r="BH12" t="n">
+        <v>0.0045687223044934555</v>
+      </c>
+      <c r="BI12" t="n">
         <v>0.0045687223044934555</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>69</v>
-      </c>
-      <c r="B13" t="s">
-        <v>112</v>
-      </c>
-      <c r="C13" t="n">
+        <v>71</v>
+      </c>
+      <c r="B13" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>114</v>
+      </c>
+      <c r="D13" t="n">
         <v>4.269833431633717</v>
       </c>
-      <c r="D13" t="n">
+      <c r="E13" t="n">
         <v>2.0233326142189574</v>
       </c>
-      <c r="E13" t="n">
+      <c r="F13" t="n">
         <v>11.150041016013201</v>
       </c>
-      <c r="F13" t="n">
+      <c r="G13" t="n">
         <v>1.4913513621177883</v>
       </c>
-      <c r="G13" t="n">
+      <c r="H13" t="n">
         <v>0.9393806962328772</v>
       </c>
-      <c r="H13" t="n">
+      <c r="I13" t="n">
         <v>2.8977925852760302</v>
       </c>
-      <c r="I13" t="n">
-        <v>0.025937678767707827</v>
-      </c>
-      <c r="J13" t="n">
-        <v>0.025937678767707827</v>
+      <c r="J13" t="e">
+        <v>#N/A</v>
       </c>
       <c r="K13" t="n">
         <v>0.025937678767707827</v>
@@ -2696,10 +2774,10 @@
         <v>0.025937678767707827</v>
       </c>
       <c r="S13" t="n">
-        <v>0.023289049619403257</v>
+        <v>0.025937678767707827</v>
       </c>
       <c r="T13" t="n">
-        <v>0.023289049619403257</v>
+        <v>0.025937678767707827</v>
       </c>
       <c r="U13" t="n">
         <v>0.023289049619403257</v>
@@ -2726,10 +2804,10 @@
         <v>0.023289049619403257</v>
       </c>
       <c r="AC13" t="n">
-        <v>0.018403957614707523</v>
+        <v>0.023289049619403257</v>
       </c>
       <c r="AD13" t="n">
-        <v>0.018403957614707523</v>
+        <v>0.023289049619403257</v>
       </c>
       <c r="AE13" t="n">
         <v>0.018403957614707523</v>
@@ -2756,10 +2834,10 @@
         <v>0.018403957614707523</v>
       </c>
       <c r="AM13" t="n">
-        <v>0.007323935049817964</v>
+        <v>0.018403957614707523</v>
       </c>
       <c r="AN13" t="n">
-        <v>0.007323935049817964</v>
+        <v>0.018403957614707523</v>
       </c>
       <c r="AO13" t="n">
         <v>0.007323935049817964</v>
@@ -2786,10 +2864,10 @@
         <v>0.007323935049817964</v>
       </c>
       <c r="AW13" t="n">
-        <v>0.004808171272136219</v>
+        <v>0.007323935049817964</v>
       </c>
       <c r="AX13" t="n">
-        <v>0.004808171272136219</v>
+        <v>0.007323935049817964</v>
       </c>
       <c r="AY13" t="n">
         <v>0.004808171272136219</v>
@@ -2816,39 +2894,45 @@
         <v>0.004808171272136219</v>
       </c>
       <c r="BG13" t="n">
+        <v>0.004808171272136219</v>
+      </c>
+      <c r="BH13" t="n">
+        <v>0.004808171272136219</v>
+      </c>
+      <c r="BI13" t="n">
         <v>0.004808171272136219</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>70</v>
-      </c>
-      <c r="B14" t="s">
-        <v>113</v>
-      </c>
-      <c r="C14" t="n">
+        <v>72</v>
+      </c>
+      <c r="B14" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="C14" t="s">
+        <v>115</v>
+      </c>
+      <c r="D14" t="n">
         <v>9.378022208852766</v>
       </c>
-      <c r="D14" t="n">
+      <c r="E14" t="n">
         <v>8.040425943414332</v>
       </c>
-      <c r="E14" t="n">
+      <c r="F14" t="n">
         <v>11.121261683844047</v>
       </c>
-      <c r="F14" t="n">
+      <c r="G14" t="n">
         <v>3.997716906210906</v>
       </c>
-      <c r="G14" t="n">
+      <c r="H14" t="n">
         <v>2.912506813304299</v>
       </c>
-      <c r="H14" t="n">
+      <c r="I14" t="n">
         <v>5.2244170102488425</v>
       </c>
-      <c r="I14" t="n">
-        <v>0.02947873448640843</v>
-      </c>
-      <c r="J14" t="n">
-        <v>0.02947873448640843</v>
+      <c r="J14" t="e">
+        <v>#N/A</v>
       </c>
       <c r="K14" t="n">
         <v>0.02947873448640843</v>
@@ -2875,10 +2959,10 @@
         <v>0.02947873448640843</v>
       </c>
       <c r="S14" t="n">
-        <v>0.017898954274626355</v>
+        <v>0.02947873448640843</v>
       </c>
       <c r="T14" t="n">
-        <v>0.017898954274626355</v>
+        <v>0.02947873448640843</v>
       </c>
       <c r="U14" t="n">
         <v>0.017898954274626355</v>
@@ -2905,10 +2989,10 @@
         <v>0.017898954274626355</v>
       </c>
       <c r="AC14" t="n">
-        <v>0.016805234876020814</v>
+        <v>0.017898954274626355</v>
       </c>
       <c r="AD14" t="n">
-        <v>0.016805234876020814</v>
+        <v>0.017898954274626355</v>
       </c>
       <c r="AE14" t="n">
         <v>0.016805234876020814</v>
@@ -2935,10 +3019,10 @@
         <v>0.016805234876020814</v>
       </c>
       <c r="AM14" t="n">
-        <v>0.016070671348514233</v>
+        <v>0.016805234876020814</v>
       </c>
       <c r="AN14" t="n">
-        <v>0.016070671348514233</v>
+        <v>0.016805234876020814</v>
       </c>
       <c r="AO14" t="n">
         <v>0.016070671348514233</v>
@@ -2965,10 +3049,10 @@
         <v>0.016070671348514233</v>
       </c>
       <c r="AW14" t="n">
-        <v>0.015397208805552065</v>
+        <v>0.016070671348514233</v>
       </c>
       <c r="AX14" t="n">
-        <v>0.015397208805552065</v>
+        <v>0.016070671348514233</v>
       </c>
       <c r="AY14" t="n">
         <v>0.015397208805552065</v>
@@ -2995,39 +3079,45 @@
         <v>0.015397208805552065</v>
       </c>
       <c r="BG14" t="n">
+        <v>0.015397208805552065</v>
+      </c>
+      <c r="BH14" t="n">
+        <v>0.015397208805552065</v>
+      </c>
+      <c r="BI14" t="n">
         <v>0.015397208805552065</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>71</v>
-      </c>
-      <c r="B15" t="s">
-        <v>114</v>
-      </c>
-      <c r="C15" t="n">
+        <v>73</v>
+      </c>
+      <c r="B15" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="C15" t="s">
+        <v>116</v>
+      </c>
+      <c r="D15" t="n">
         <v>9.453775134856752</v>
       </c>
-      <c r="D15" t="n">
+      <c r="E15" t="n">
         <v>5.141618475417184</v>
       </c>
-      <c r="E15" t="n">
+      <c r="F15" t="n">
         <v>14.363909030978709</v>
       </c>
-      <c r="F15" t="n">
+      <c r="G15" t="n">
         <v>2.363286707312858</v>
       </c>
-      <c r="G15" t="n">
+      <c r="H15" t="n">
         <v>1.3153986716230488</v>
       </c>
-      <c r="H15" t="n">
+      <c r="I15" t="n">
         <v>4.319129488813189</v>
       </c>
-      <c r="I15" t="n">
-        <v>0.011240736529343476</v>
-      </c>
-      <c r="J15" t="n">
-        <v>0.011240736529343476</v>
+      <c r="J15" t="e">
+        <v>#N/A</v>
       </c>
       <c r="K15" t="n">
         <v>0.011240736529343476</v>
@@ -3054,10 +3144,10 @@
         <v>0.011240736529343476</v>
       </c>
       <c r="S15" t="n">
-        <v>0.006632000307533126</v>
+        <v>0.011240736529343476</v>
       </c>
       <c r="T15" t="n">
-        <v>0.006632000307533126</v>
+        <v>0.011240736529343476</v>
       </c>
       <c r="U15" t="n">
         <v>0.006632000307533126</v>
@@ -3084,10 +3174,10 @@
         <v>0.006632000307533126</v>
       </c>
       <c r="AC15" t="n">
-        <v>0.005758520253007405</v>
+        <v>0.006632000307533126</v>
       </c>
       <c r="AD15" t="n">
-        <v>0.005758520253007405</v>
+        <v>0.006632000307533126</v>
       </c>
       <c r="AE15" t="n">
         <v>0.005758520253007405</v>
@@ -3114,10 +3204,10 @@
         <v>0.005758520253007405</v>
       </c>
       <c r="AM15" t="n">
-        <v>0.005592314195117298</v>
+        <v>0.005758520253007405</v>
       </c>
       <c r="AN15" t="n">
-        <v>0.005592314195117298</v>
+        <v>0.005758520253007405</v>
       </c>
       <c r="AO15" t="n">
         <v>0.005592314195117298</v>
@@ -3144,10 +3234,10 @@
         <v>0.005592314195117298</v>
       </c>
       <c r="AW15" t="n">
-        <v>0.005451273429188141</v>
+        <v>0.005592314195117298</v>
       </c>
       <c r="AX15" t="n">
-        <v>0.005451273429188141</v>
+        <v>0.005592314195117298</v>
       </c>
       <c r="AY15" t="n">
         <v>0.005451273429188141</v>
@@ -3174,39 +3264,45 @@
         <v>0.005451273429188141</v>
       </c>
       <c r="BG15" t="n">
+        <v>0.005451273429188141</v>
+      </c>
+      <c r="BH15" t="n">
+        <v>0.005451273429188141</v>
+      </c>
+      <c r="BI15" t="n">
         <v>0.005451273429188141</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>72</v>
-      </c>
-      <c r="B16" t="s">
-        <v>115</v>
-      </c>
-      <c r="C16" t="n">
+        <v>74</v>
+      </c>
+      <c r="B16" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="C16" t="s">
+        <v>117</v>
+      </c>
+      <c r="D16" t="n">
         <v>7.890096556921813</v>
       </c>
-      <c r="D16" t="n">
+      <c r="E16" t="n">
         <v>7.238221457163206</v>
       </c>
-      <c r="E16" t="n">
+      <c r="F16" t="n">
         <v>8.53841961215986</v>
       </c>
-      <c r="F16" t="n">
+      <c r="G16" t="n">
         <v>1.8630379794744352</v>
       </c>
-      <c r="G16" t="n">
+      <c r="H16" t="n">
         <v>1.2570581131559502</v>
       </c>
-      <c r="H16" t="n">
+      <c r="I16" t="n">
         <v>2.488874292667167</v>
       </c>
-      <c r="I16" t="n">
-        <v>0.0036421944130116124</v>
-      </c>
-      <c r="J16" t="n">
-        <v>0.0036421944130116124</v>
+      <c r="J16" t="e">
+        <v>#N/A</v>
       </c>
       <c r="K16" t="n">
         <v>0.0036421944130116124</v>
@@ -3233,10 +3329,10 @@
         <v>0.0036421944130116124</v>
       </c>
       <c r="S16" t="n">
-        <v>0.003593691184398118</v>
+        <v>0.0036421944130116124</v>
       </c>
       <c r="T16" t="n">
-        <v>0.003593691184398118</v>
+        <v>0.0036421944130116124</v>
       </c>
       <c r="U16" t="n">
         <v>0.003593691184398118</v>
@@ -3263,10 +3359,10 @@
         <v>0.003593691184398118</v>
       </c>
       <c r="AC16" t="n">
-        <v>0.0035450033341567267</v>
+        <v>0.003593691184398118</v>
       </c>
       <c r="AD16" t="n">
-        <v>0.0035450033341567267</v>
+        <v>0.003593691184398118</v>
       </c>
       <c r="AE16" t="n">
         <v>0.0035450033341567267</v>
@@ -3293,10 +3389,10 @@
         <v>0.0035450033341567267</v>
       </c>
       <c r="AM16" t="n">
-        <v>0.003493027184231412</v>
+        <v>0.0035450033341567267</v>
       </c>
       <c r="AN16" t="n">
-        <v>0.003493027184231412</v>
+        <v>0.0035450033341567267</v>
       </c>
       <c r="AO16" t="n">
         <v>0.003493027184231412</v>
@@ -3323,10 +3419,10 @@
         <v>0.003493027184231412</v>
       </c>
       <c r="AW16" t="n">
-        <v>0.0034418194669544543</v>
+        <v>0.003493027184231412</v>
       </c>
       <c r="AX16" t="n">
-        <v>0.0034418194669544543</v>
+        <v>0.003493027184231412</v>
       </c>
       <c r="AY16" t="n">
         <v>0.0034418194669544543</v>
@@ -3353,39 +3449,45 @@
         <v>0.0034418194669544543</v>
       </c>
       <c r="BG16" t="n">
+        <v>0.0034418194669544543</v>
+      </c>
+      <c r="BH16" t="n">
+        <v>0.0034418194669544543</v>
+      </c>
+      <c r="BI16" t="n">
         <v>0.0034418194669544543</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>73</v>
-      </c>
-      <c r="B17" t="s">
-        <v>116</v>
-      </c>
-      <c r="C17" t="n">
+        <v>75</v>
+      </c>
+      <c r="B17" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="C17" t="s">
+        <v>118</v>
+      </c>
+      <c r="D17" t="n">
         <v>21.396646963748402</v>
       </c>
-      <c r="D17" t="n">
+      <c r="E17" t="n">
         <v>19.684766619044858</v>
       </c>
-      <c r="E17" t="n">
+      <c r="F17" t="n">
         <v>22.925130788703967</v>
       </c>
-      <c r="F17" t="n">
+      <c r="G17" t="n">
         <v>7.356499124639927</v>
       </c>
-      <c r="G17" t="n">
+      <c r="H17" t="n">
         <v>5.287293829799609</v>
       </c>
-      <c r="H17" t="n">
+      <c r="I17" t="n">
         <v>13.810200028477123</v>
       </c>
-      <c r="I17" t="n">
-        <v>0.006070511964195546</v>
-      </c>
-      <c r="J17" t="n">
-        <v>0.006070511964195546</v>
+      <c r="J17" t="e">
+        <v>#N/A</v>
       </c>
       <c r="K17" t="n">
         <v>0.006070511964195546</v>
@@ -3412,10 +3514,10 @@
         <v>0.006070511964195546</v>
       </c>
       <c r="S17" t="n">
-        <v>0.006045866336362593</v>
+        <v>0.006070511964195546</v>
       </c>
       <c r="T17" t="n">
-        <v>0.006045866336362593</v>
+        <v>0.006070511964195546</v>
       </c>
       <c r="U17" t="n">
         <v>0.006045866336362593</v>
@@ -3442,10 +3544,10 @@
         <v>0.006045866336362593</v>
       </c>
       <c r="AC17" t="n">
-        <v>0.006021315224901258</v>
+        <v>0.006045866336362593</v>
       </c>
       <c r="AD17" t="n">
-        <v>0.006021315224901258</v>
+        <v>0.006045866336362593</v>
       </c>
       <c r="AE17" t="n">
         <v>0.006021315224901258</v>
@@ -3472,10 +3574,10 @@
         <v>0.006021315224901258</v>
       </c>
       <c r="AM17" t="n">
-        <v>0.0059968582686869</v>
+        <v>0.006021315224901258</v>
       </c>
       <c r="AN17" t="n">
-        <v>0.0059968582686869</v>
+        <v>0.006021315224901258</v>
       </c>
       <c r="AO17" t="n">
         <v>0.0059968582686869</v>
@@ -3502,10 +3604,10 @@
         <v>0.0059968582686869</v>
       </c>
       <c r="AW17" t="n">
-        <v>0.005972495327723593</v>
+        <v>0.0059968582686869</v>
       </c>
       <c r="AX17" t="n">
-        <v>0.005972495327723593</v>
+        <v>0.0059968582686869</v>
       </c>
       <c r="AY17" t="n">
         <v>0.005972495327723593</v>
@@ -3532,39 +3634,45 @@
         <v>0.005972495327723593</v>
       </c>
       <c r="BG17" t="n">
+        <v>0.005972495327723593</v>
+      </c>
+      <c r="BH17" t="n">
+        <v>0.005972495327723593</v>
+      </c>
+      <c r="BI17" t="n">
         <v>0.005972495327723593</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>74</v>
-      </c>
-      <c r="B18" t="s">
-        <v>117</v>
-      </c>
-      <c r="C18" t="n">
+        <v>76</v>
+      </c>
+      <c r="B18" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="C18" t="s">
+        <v>119</v>
+      </c>
+      <c r="D18" t="n">
         <v>21.39592852731933</v>
       </c>
-      <c r="D18" t="n">
+      <c r="E18" t="n">
         <v>21.150918385281763</v>
       </c>
-      <c r="E18" t="n">
+      <c r="F18" t="n">
         <v>21.653204886808528</v>
       </c>
-      <c r="F18" t="n">
+      <c r="G18" t="n">
         <v>5.040246871274304</v>
       </c>
-      <c r="G18" t="n">
+      <c r="H18" t="n">
         <v>3.714297918249544</v>
       </c>
-      <c r="H18" t="n">
+      <c r="I18" t="n">
         <v>6.433834176695067</v>
       </c>
-      <c r="I18" t="n">
-        <v>0.003526948081399617</v>
-      </c>
-      <c r="J18" t="n">
-        <v>0.003526948081399617</v>
+      <c r="J18" t="e">
+        <v>#N/A</v>
       </c>
       <c r="K18" t="n">
         <v>0.003526948081399617</v>
@@ -3591,10 +3699,10 @@
         <v>0.003526948081399617</v>
       </c>
       <c r="S18" t="n">
-        <v>0.00350972742460236</v>
+        <v>0.003526948081399617</v>
       </c>
       <c r="T18" t="n">
-        <v>0.00350972742460236</v>
+        <v>0.003526948081399617</v>
       </c>
       <c r="U18" t="n">
         <v>0.00350972742460236</v>
@@ -3621,10 +3729,10 @@
         <v>0.00350972742460236</v>
       </c>
       <c r="AC18" t="n">
-        <v>0.003492590849578825</v>
+        <v>0.00350972742460236</v>
       </c>
       <c r="AD18" t="n">
-        <v>0.003492590849578825</v>
+        <v>0.00350972742460236</v>
       </c>
       <c r="AE18" t="n">
         <v>0.003492590849578825</v>
@@ -3651,10 +3759,10 @@
         <v>0.003492590849578825</v>
       </c>
       <c r="AM18" t="n">
-        <v>0.003475537945789142</v>
+        <v>0.003492590849578825</v>
       </c>
       <c r="AN18" t="n">
-        <v>0.003475537945789142</v>
+        <v>0.003492590849578825</v>
       </c>
       <c r="AO18" t="n">
         <v>0.003475537945789142</v>
@@ -3681,10 +3789,10 @@
         <v>0.003475537945789142</v>
       </c>
       <c r="AW18" t="n">
-        <v>0.0034585683046964633</v>
+        <v>0.003475537945789142</v>
       </c>
       <c r="AX18" t="n">
-        <v>0.0034585683046964633</v>
+        <v>0.003475537945789142</v>
       </c>
       <c r="AY18" t="n">
         <v>0.0034585683046964633</v>
@@ -3711,39 +3819,45 @@
         <v>0.0034585683046964633</v>
       </c>
       <c r="BG18" t="n">
+        <v>0.0034585683046964633</v>
+      </c>
+      <c r="BH18" t="n">
+        <v>0.0034585683046964633</v>
+      </c>
+      <c r="BI18" t="n">
         <v>0.0034585683046964633</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>75</v>
-      </c>
-      <c r="B19" t="s">
-        <v>118</v>
-      </c>
-      <c r="C19" t="n">
+        <v>77</v>
+      </c>
+      <c r="B19" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="C19" t="s">
+        <v>120</v>
+      </c>
+      <c r="D19" t="n">
         <v>1.4450053656102577</v>
       </c>
-      <c r="D19" t="n">
+      <c r="E19" t="n">
         <v>1.1504192623496707</v>
       </c>
-      <c r="E19" t="n">
+      <c r="F19" t="n">
         <v>2.0460970615376115</v>
       </c>
-      <c r="F19" t="n">
+      <c r="G19" t="n">
         <v>1.1305394562005169</v>
       </c>
-      <c r="G19" t="n">
+      <c r="H19" t="n">
         <v>0.8367711151646469</v>
       </c>
-      <c r="H19" t="n">
+      <c r="I19" t="n">
         <v>1.6941656791684105</v>
       </c>
-      <c r="I19" t="n">
-        <v>0.028436760026489795</v>
-      </c>
-      <c r="J19" t="n">
-        <v>0.028436760026489795</v>
+      <c r="J19" t="e">
+        <v>#N/A</v>
       </c>
       <c r="K19" t="n">
         <v>0.028436760026489795</v>
@@ -3770,10 +3884,10 @@
         <v>0.028436760026489795</v>
       </c>
       <c r="S19" t="n">
-        <v>0.021260975968258034</v>
+        <v>0.028436760026489795</v>
       </c>
       <c r="T19" t="n">
-        <v>0.021260975968258034</v>
+        <v>0.028436760026489795</v>
       </c>
       <c r="U19" t="n">
         <v>0.021260975968258034</v>
@@ -3800,10 +3914,10 @@
         <v>0.021260975968258034</v>
       </c>
       <c r="AC19" t="n">
-        <v>0.01571108571664845</v>
+        <v>0.021260975968258034</v>
       </c>
       <c r="AD19" t="n">
-        <v>0.01571108571664845</v>
+        <v>0.021260975968258034</v>
       </c>
       <c r="AE19" t="n">
         <v>0.01571108571664845</v>
@@ -3830,10 +3944,10 @@
         <v>0.01571108571664845</v>
       </c>
       <c r="AM19" t="n">
-        <v>0.011893774595088308</v>
+        <v>0.01571108571664845</v>
       </c>
       <c r="AN19" t="n">
-        <v>0.011893774595088308</v>
+        <v>0.01571108571664845</v>
       </c>
       <c r="AO19" t="n">
         <v>0.011893774595088308</v>
@@ -3860,10 +3974,10 @@
         <v>0.011893774595088308</v>
       </c>
       <c r="AW19" t="n">
-        <v>0.00881322350246722</v>
+        <v>0.011893774595088308</v>
       </c>
       <c r="AX19" t="n">
-        <v>0.00881322350246722</v>
+        <v>0.011893774595088308</v>
       </c>
       <c r="AY19" t="n">
         <v>0.00881322350246722</v>
@@ -3890,39 +4004,45 @@
         <v>0.00881322350246722</v>
       </c>
       <c r="BG19" t="n">
+        <v>0.00881322350246722</v>
+      </c>
+      <c r="BH19" t="n">
+        <v>0.00881322350246722</v>
+      </c>
+      <c r="BI19" t="n">
         <v>0.00881322350246722</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>76</v>
-      </c>
-      <c r="B20" t="s">
-        <v>119</v>
-      </c>
-      <c r="C20" t="n">
+        <v>78</v>
+      </c>
+      <c r="B20" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="C20" t="s">
+        <v>121</v>
+      </c>
+      <c r="D20" t="n">
         <v>18.382277000825134</v>
       </c>
-      <c r="D20" t="n">
+      <c r="E20" t="n">
         <v>17.539571339867503</v>
       </c>
-      <c r="E20" t="n">
+      <c r="F20" t="n">
         <v>19.2291751087374</v>
       </c>
-      <c r="F20" t="n">
+      <c r="G20" t="n">
         <v>5.056079166487359</v>
       </c>
-      <c r="G20" t="n">
+      <c r="H20" t="n">
         <v>3.9149310147345924</v>
       </c>
-      <c r="H20" t="n">
+      <c r="I20" t="n">
         <v>6.373609205620845</v>
       </c>
-      <c r="I20" t="n">
-        <v>0.010905393238831884</v>
-      </c>
-      <c r="J20" t="n">
-        <v>0.010905393238831884</v>
+      <c r="J20" t="e">
+        <v>#N/A</v>
       </c>
       <c r="K20" t="n">
         <v>0.010905393238831884</v>
@@ -3949,10 +4069,10 @@
         <v>0.010905393238831884</v>
       </c>
       <c r="S20" t="n">
-        <v>0.01072431054493137</v>
+        <v>0.010905393238831884</v>
       </c>
       <c r="T20" t="n">
-        <v>0.01072431054493137</v>
+        <v>0.010905393238831884</v>
       </c>
       <c r="U20" t="n">
         <v>0.01072431054493137</v>
@@ -3979,10 +4099,10 @@
         <v>0.01072431054493137</v>
       </c>
       <c r="AC20" t="n">
-        <v>0.010545805579428524</v>
+        <v>0.01072431054493137</v>
       </c>
       <c r="AD20" t="n">
-        <v>0.010545805579428524</v>
+        <v>0.01072431054493137</v>
       </c>
       <c r="AE20" t="n">
         <v>0.010545805579428524</v>
@@ -4009,10 +4129,10 @@
         <v>0.010545805579428524</v>
       </c>
       <c r="AM20" t="n">
-        <v>0.010366782915033923</v>
+        <v>0.010545805579428524</v>
       </c>
       <c r="AN20" t="n">
-        <v>0.010366782915033923</v>
+        <v>0.010545805579428524</v>
       </c>
       <c r="AO20" t="n">
         <v>0.010366782915033923</v>
@@ -4039,10 +4159,10 @@
         <v>0.010366782915033923</v>
       </c>
       <c r="AW20" t="n">
-        <v>0.010184365120387362</v>
+        <v>0.010366782915033923</v>
       </c>
       <c r="AX20" t="n">
-        <v>0.010184365120387362</v>
+        <v>0.010366782915033923</v>
       </c>
       <c r="AY20" t="n">
         <v>0.010184365120387362</v>
@@ -4069,39 +4189,45 @@
         <v>0.010184365120387362</v>
       </c>
       <c r="BG20" t="n">
+        <v>0.010184365120387362</v>
+      </c>
+      <c r="BH20" t="n">
+        <v>0.010184365120387362</v>
+      </c>
+      <c r="BI20" t="n">
         <v>0.010184365120387362</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>77</v>
-      </c>
-      <c r="B21" t="s">
-        <v>120</v>
-      </c>
-      <c r="C21" t="n">
+        <v>79</v>
+      </c>
+      <c r="B21" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="C21" t="s">
+        <v>122</v>
+      </c>
+      <c r="D21" t="n">
         <v>14.421914306384876</v>
       </c>
-      <c r="D21" t="n">
+      <c r="E21" t="n">
         <v>13.125122070741808</v>
       </c>
-      <c r="E21" t="n">
+      <c r="F21" t="n">
         <v>15.635849822406538</v>
       </c>
-      <c r="F21" t="n">
+      <c r="G21" t="n">
         <v>4.130481534728691</v>
       </c>
-      <c r="G21" t="n">
+      <c r="H21" t="n">
         <v>2.826582073861523</v>
       </c>
-      <c r="H21" t="n">
+      <c r="I21" t="n">
         <v>5.16582327228604</v>
       </c>
-      <c r="I21" t="n">
-        <v>0.010779048028423688</v>
-      </c>
-      <c r="J21" t="n">
-        <v>0.010779048028423688</v>
+      <c r="J21" t="e">
+        <v>#N/A</v>
       </c>
       <c r="K21" t="n">
         <v>0.010779048028423688</v>
@@ -4128,10 +4254,10 @@
         <v>0.010779048028423688</v>
       </c>
       <c r="S21" t="n">
-        <v>0.010539572637739792</v>
+        <v>0.010779048028423688</v>
       </c>
       <c r="T21" t="n">
-        <v>0.010539572637739792</v>
+        <v>0.010779048028423688</v>
       </c>
       <c r="U21" t="n">
         <v>0.010539572637739792</v>
@@ -4158,10 +4284,10 @@
         <v>0.010539572637739792</v>
       </c>
       <c r="AC21" t="n">
-        <v>0.010305007879921746</v>
+        <v>0.010539572637739792</v>
       </c>
       <c r="AD21" t="n">
-        <v>0.010305007879921746</v>
+        <v>0.010539572637739792</v>
       </c>
       <c r="AE21" t="n">
         <v>0.010305007879921746</v>
@@ -4188,10 +4314,10 @@
         <v>0.010305007879921746</v>
       </c>
       <c r="AM21" t="n">
-        <v>0.010080198212492241</v>
+        <v>0.010305007879921746</v>
       </c>
       <c r="AN21" t="n">
-        <v>0.010080198212492241</v>
+        <v>0.010305007879921746</v>
       </c>
       <c r="AO21" t="n">
         <v>0.010080198212492241</v>
@@ -4218,10 +4344,10 @@
         <v>0.010080198212492241</v>
       </c>
       <c r="AW21" t="n">
-        <v>0.00985988516569396</v>
+        <v>0.010080198212492241</v>
       </c>
       <c r="AX21" t="n">
-        <v>0.00985988516569396</v>
+        <v>0.010080198212492241</v>
       </c>
       <c r="AY21" t="n">
         <v>0.00985988516569396</v>
@@ -4248,39 +4374,45 @@
         <v>0.00985988516569396</v>
       </c>
       <c r="BG21" t="n">
+        <v>0.00985988516569396</v>
+      </c>
+      <c r="BH21" t="n">
+        <v>0.00985988516569396</v>
+      </c>
+      <c r="BI21" t="n">
         <v>0.00985988516569396</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>78</v>
-      </c>
-      <c r="B22" t="s">
-        <v>121</v>
-      </c>
-      <c r="C22" t="n">
+        <v>80</v>
+      </c>
+      <c r="B22" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="C22" t="s">
+        <v>123</v>
+      </c>
+      <c r="D22" t="n">
         <v>11.036976146829996</v>
       </c>
-      <c r="D22" t="n">
+      <c r="E22" t="n">
         <v>9.670447345953452</v>
       </c>
-      <c r="E22" t="n">
+      <c r="F22" t="n">
         <v>12.320234813105095</v>
       </c>
-      <c r="F22" t="n">
+      <c r="G22" t="n">
         <v>6.1238731543784075</v>
       </c>
-      <c r="G22" t="n">
+      <c r="H22" t="n">
         <v>3.724265351958743</v>
       </c>
-      <c r="H22" t="n">
+      <c r="I22" t="n">
         <v>8.307583685287176</v>
       </c>
-      <c r="I22" t="n">
-        <v>0.0266784655849011</v>
-      </c>
-      <c r="J22" t="n">
-        <v>0.0266784655849011</v>
+      <c r="J22" t="e">
+        <v>#N/A</v>
       </c>
       <c r="K22" t="n">
         <v>0.0266784655849011</v>
@@ -4307,10 +4439,10 @@
         <v>0.0266784655849011</v>
       </c>
       <c r="S22" t="n">
-        <v>0.02556653211274984</v>
+        <v>0.0266784655849011</v>
       </c>
       <c r="T22" t="n">
-        <v>0.02556653211274984</v>
+        <v>0.0266784655849011</v>
       </c>
       <c r="U22" t="n">
         <v>0.02556653211274984</v>
@@ -4337,10 +4469,10 @@
         <v>0.02556653211274984</v>
       </c>
       <c r="AC22" t="n">
-        <v>0.024499597145898822</v>
+        <v>0.02556653211274984</v>
       </c>
       <c r="AD22" t="n">
-        <v>0.024499597145898822</v>
+        <v>0.02556653211274984</v>
       </c>
       <c r="AE22" t="n">
         <v>0.024499597145898822</v>
@@ -4367,10 +4499,10 @@
         <v>0.024499597145898822</v>
       </c>
       <c r="AM22" t="n">
-        <v>0.02347586195742126</v>
+        <v>0.024499597145898822</v>
       </c>
       <c r="AN22" t="n">
-        <v>0.02347586195742126</v>
+        <v>0.024499597145898822</v>
       </c>
       <c r="AO22" t="n">
         <v>0.02347586195742126</v>
@@ -4397,10 +4529,10 @@
         <v>0.02347586195742126</v>
       </c>
       <c r="AW22" t="n">
-        <v>0.02249362818879517</v>
+        <v>0.02347586195742126</v>
       </c>
       <c r="AX22" t="n">
-        <v>0.02249362818879517</v>
+        <v>0.02347586195742126</v>
       </c>
       <c r="AY22" t="n">
         <v>0.02249362818879517</v>
@@ -4427,39 +4559,45 @@
         <v>0.02249362818879517</v>
       </c>
       <c r="BG22" t="n">
+        <v>0.02249362818879517</v>
+      </c>
+      <c r="BH22" t="n">
+        <v>0.02249362818879517</v>
+      </c>
+      <c r="BI22" t="n">
         <v>0.02249362818879517</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>79</v>
-      </c>
-      <c r="B23" t="s">
-        <v>122</v>
-      </c>
-      <c r="C23" t="n">
+        <v>81</v>
+      </c>
+      <c r="B23" t="n">
+        <v>22.0</v>
+      </c>
+      <c r="C23" t="s">
+        <v>124</v>
+      </c>
+      <c r="D23" t="n">
         <v>9.029355460219683</v>
       </c>
-      <c r="D23" t="n">
+      <c r="E23" t="n">
         <v>8.541652343228233</v>
       </c>
-      <c r="E23" t="n">
+      <c r="F23" t="n">
         <v>9.462110037842205</v>
       </c>
-      <c r="F23" t="n">
+      <c r="G23" t="n">
         <v>3.095953724671635</v>
       </c>
-      <c r="G23" t="n">
+      <c r="H23" t="n">
         <v>2.629782205623947</v>
       </c>
-      <c r="H23" t="n">
+      <c r="I23" t="n">
         <v>3.542896955724509</v>
       </c>
-      <c r="I23" t="n">
-        <v>0.014114018642574421</v>
-      </c>
-      <c r="J23" t="n">
-        <v>0.014114018642574421</v>
+      <c r="J23" t="e">
+        <v>#N/A</v>
       </c>
       <c r="K23" t="n">
         <v>0.014114018642574421</v>
@@ -4486,10 +4624,10 @@
         <v>0.014114018642574421</v>
       </c>
       <c r="S23" t="n">
-        <v>0.013518444204261737</v>
+        <v>0.014114018642574421</v>
       </c>
       <c r="T23" t="n">
-        <v>0.013518444204261737</v>
+        <v>0.014114018642574421</v>
       </c>
       <c r="U23" t="n">
         <v>0.013518444204261737</v>
@@ -4516,10 +4654,10 @@
         <v>0.013518444204261737</v>
       </c>
       <c r="AC23" t="n">
-        <v>0.012947109696753589</v>
+        <v>0.013518444204261737</v>
       </c>
       <c r="AD23" t="n">
-        <v>0.012947109696753589</v>
+        <v>0.013518444204261737</v>
       </c>
       <c r="AE23" t="n">
         <v>0.012947109696753589</v>
@@ -4546,10 +4684,10 @@
         <v>0.012947109696753589</v>
       </c>
       <c r="AM23" t="n">
-        <v>0.012398724721505338</v>
+        <v>0.012947109696753589</v>
       </c>
       <c r="AN23" t="n">
-        <v>0.012398724721505338</v>
+        <v>0.012947109696753589</v>
       </c>
       <c r="AO23" t="n">
         <v>0.012398724721505338</v>
@@ -4576,10 +4714,10 @@
         <v>0.012398724721505338</v>
       </c>
       <c r="AW23" t="n">
-        <v>0.011870229464803294</v>
+        <v>0.012398724721505338</v>
       </c>
       <c r="AX23" t="n">
-        <v>0.011870229464803294</v>
+        <v>0.012398724721505338</v>
       </c>
       <c r="AY23" t="n">
         <v>0.011870229464803294</v>
@@ -4606,39 +4744,45 @@
         <v>0.011870229464803294</v>
       </c>
       <c r="BG23" t="n">
+        <v>0.011870229464803294</v>
+      </c>
+      <c r="BH23" t="n">
+        <v>0.011870229464803294</v>
+      </c>
+      <c r="BI23" t="n">
         <v>0.011870229464803294</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>80</v>
-      </c>
-      <c r="B24" t="s">
-        <v>123</v>
-      </c>
-      <c r="C24" t="n">
+        <v>82</v>
+      </c>
+      <c r="B24" t="n">
+        <v>23.0</v>
+      </c>
+      <c r="C24" t="s">
+        <v>125</v>
+      </c>
+      <c r="D24" t="n">
         <v>11.561269812751254</v>
       </c>
-      <c r="D24" t="n">
+      <c r="E24" t="n">
         <v>10.380660432078193</v>
       </c>
-      <c r="E24" t="n">
+      <c r="F24" t="n">
         <v>12.517564227439182</v>
       </c>
-      <c r="F24" t="n">
+      <c r="G24" t="n">
         <v>5.849016373000321</v>
       </c>
-      <c r="G24" t="n">
+      <c r="H24" t="n">
         <v>5.40621716665606</v>
       </c>
-      <c r="H24" t="n">
+      <c r="I24" t="n">
         <v>6.305563421814043</v>
       </c>
-      <c r="I24" t="n">
-        <v>0.0274899668886567</v>
-      </c>
-      <c r="J24" t="n">
-        <v>0.0274899668886567</v>
+      <c r="J24" t="e">
+        <v>#N/A</v>
       </c>
       <c r="K24" t="n">
         <v>0.0274899668886567</v>
@@ -4665,10 +4809,10 @@
         <v>0.0274899668886567</v>
       </c>
       <c r="S24" t="n">
-        <v>0.026290934141350242</v>
+        <v>0.0274899668886567</v>
       </c>
       <c r="T24" t="n">
-        <v>0.026290934141350242</v>
+        <v>0.0274899668886567</v>
       </c>
       <c r="U24" t="n">
         <v>0.026290934141350242</v>
@@ -4695,10 +4839,10 @@
         <v>0.026290934141350242</v>
       </c>
       <c r="AC24" t="n">
-        <v>0.025143061057131356</v>
+        <v>0.026290934141350242</v>
       </c>
       <c r="AD24" t="n">
-        <v>0.025143061057131356</v>
+        <v>0.026290934141350242</v>
       </c>
       <c r="AE24" t="n">
         <v>0.025143061057131356</v>
@@ -4725,10 +4869,10 @@
         <v>0.025143061057131356</v>
       </c>
       <c r="AM24" t="n">
-        <v>0.024072588450136045</v>
+        <v>0.025143061057131356</v>
       </c>
       <c r="AN24" t="n">
-        <v>0.024072588450136045</v>
+        <v>0.025143061057131356</v>
       </c>
       <c r="AO24" t="n">
         <v>0.024072588450136045</v>
@@ -4755,10 +4899,10 @@
         <v>0.024072588450136045</v>
       </c>
       <c r="AW24" t="n">
-        <v>0.02304602217809366</v>
+        <v>0.024072588450136045</v>
       </c>
       <c r="AX24" t="n">
-        <v>0.02304602217809366</v>
+        <v>0.024072588450136045</v>
       </c>
       <c r="AY24" t="n">
         <v>0.02304602217809366</v>
@@ -4785,39 +4929,45 @@
         <v>0.02304602217809366</v>
       </c>
       <c r="BG24" t="n">
+        <v>0.02304602217809366</v>
+      </c>
+      <c r="BH24" t="n">
+        <v>0.02304602217809366</v>
+      </c>
+      <c r="BI24" t="n">
         <v>0.02304602217809366</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>81</v>
-      </c>
-      <c r="B25" t="s">
-        <v>124</v>
-      </c>
-      <c r="C25" t="n">
+        <v>83</v>
+      </c>
+      <c r="B25" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="C25" t="s">
+        <v>126</v>
+      </c>
+      <c r="D25" t="n">
         <v>15.046611794838846</v>
       </c>
-      <c r="D25" t="n">
+      <c r="E25" t="n">
         <v>14.386405963688468</v>
       </c>
-      <c r="E25" t="n">
+      <c r="F25" t="n">
         <v>15.797329576847236</v>
       </c>
-      <c r="F25" t="n">
+      <c r="G25" t="n">
         <v>2.9781698047932634</v>
       </c>
-      <c r="G25" t="n">
+      <c r="H25" t="n">
         <v>2.013025584078103</v>
       </c>
-      <c r="H25" t="n">
+      <c r="I25" t="n">
         <v>4.087847787067009</v>
       </c>
-      <c r="I25" t="n">
-        <v>0.005029211096501918</v>
-      </c>
-      <c r="J25" t="n">
-        <v>0.005029211096501918</v>
+      <c r="J25" t="e">
+        <v>#N/A</v>
       </c>
       <c r="K25" t="n">
         <v>0.005029211096501918</v>
@@ -4844,10 +4994,10 @@
         <v>0.005029211096501918</v>
       </c>
       <c r="S25" t="n">
-        <v>0.004961793512282675</v>
+        <v>0.005029211096501918</v>
       </c>
       <c r="T25" t="n">
-        <v>0.004961793512282675</v>
+        <v>0.005029211096501918</v>
       </c>
       <c r="U25" t="n">
         <v>0.004961793512282675</v>
@@ -4874,10 +5024,10 @@
         <v>0.004961793512282675</v>
       </c>
       <c r="AC25" t="n">
-        <v>0.00500012191827901</v>
+        <v>0.004961793512282675</v>
       </c>
       <c r="AD25" t="n">
-        <v>0.00500012191827901</v>
+        <v>0.004961793512282675</v>
       </c>
       <c r="AE25" t="n">
         <v>0.00500012191827901</v>
@@ -4904,10 +5054,10 @@
         <v>0.00500012191827901</v>
       </c>
       <c r="AM25" t="n">
-        <v>0.005055966343001384</v>
+        <v>0.00500012191827901</v>
       </c>
       <c r="AN25" t="n">
-        <v>0.005055966343001384</v>
+        <v>0.00500012191827901</v>
       </c>
       <c r="AO25" t="n">
         <v>0.005055966343001384</v>
@@ -4934,10 +5084,10 @@
         <v>0.005055966343001384</v>
       </c>
       <c r="AW25" t="n">
-        <v>0.00496353488385024</v>
+        <v>0.005055966343001384</v>
       </c>
       <c r="AX25" t="n">
-        <v>0.00496353488385024</v>
+        <v>0.005055966343001384</v>
       </c>
       <c r="AY25" t="n">
         <v>0.00496353488385024</v>
@@ -4964,39 +5114,45 @@
         <v>0.00496353488385024</v>
       </c>
       <c r="BG25" t="n">
+        <v>0.00496353488385024</v>
+      </c>
+      <c r="BH25" t="n">
+        <v>0.00496353488385024</v>
+      </c>
+      <c r="BI25" t="n">
         <v>0.00496353488385024</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>82</v>
-      </c>
-      <c r="B26" t="s">
-        <v>125</v>
-      </c>
-      <c r="C26" t="n">
+        <v>84</v>
+      </c>
+      <c r="B26" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="C26" t="s">
+        <v>127</v>
+      </c>
+      <c r="D26" t="n">
         <v>8.154828116384149</v>
       </c>
-      <c r="D26" t="n">
+      <c r="E26" t="n">
         <v>7.55630349268316</v>
       </c>
-      <c r="E26" t="n">
+      <c r="F26" t="n">
         <v>8.811694521321126</v>
       </c>
-      <c r="F26" t="n">
+      <c r="G26" t="n">
         <v>1.7140777673390613</v>
       </c>
-      <c r="G26" t="n">
+      <c r="H26" t="n">
         <v>1.0216484339721978</v>
       </c>
-      <c r="H26" t="n">
+      <c r="I26" t="n">
         <v>2.3655135149839004</v>
       </c>
-      <c r="I26" t="n">
-        <v>0.0047417415448028685</v>
-      </c>
-      <c r="J26" t="n">
-        <v>0.0047417415448028685</v>
+      <c r="J26" t="e">
+        <v>#N/A</v>
       </c>
       <c r="K26" t="n">
         <v>0.0047417415448028685</v>
@@ -5023,10 +5179,10 @@
         <v>0.0047417415448028685</v>
       </c>
       <c r="S26" t="n">
-        <v>0.004618470001659425</v>
+        <v>0.0047417415448028685</v>
       </c>
       <c r="T26" t="n">
-        <v>0.004618470001659425</v>
+        <v>0.0047417415448028685</v>
       </c>
       <c r="U26" t="n">
         <v>0.004618470001659425</v>
@@ -5053,10 +5209,10 @@
         <v>0.004618470001659425</v>
       </c>
       <c r="AC26" t="n">
-        <v>0.004496007287574466</v>
+        <v>0.004618470001659425</v>
       </c>
       <c r="AD26" t="n">
-        <v>0.004496007287574466</v>
+        <v>0.004618470001659425</v>
       </c>
       <c r="AE26" t="n">
         <v>0.004496007287574466</v>
@@ -5083,10 +5239,10 @@
         <v>0.004496007287574466</v>
       </c>
       <c r="AM26" t="n">
-        <v>0.0043823452434456735</v>
+        <v>0.004496007287574466</v>
       </c>
       <c r="AN26" t="n">
-        <v>0.0043823452434456735</v>
+        <v>0.004496007287574466</v>
       </c>
       <c r="AO26" t="n">
         <v>0.0043823452434456735</v>
@@ -5113,10 +5269,10 @@
         <v>0.0043823452434456735</v>
       </c>
       <c r="AW26" t="n">
-        <v>0.004271104949584448</v>
+        <v>0.0043823452434456735</v>
       </c>
       <c r="AX26" t="n">
-        <v>0.004271104949584448</v>
+        <v>0.0043823452434456735</v>
       </c>
       <c r="AY26" t="n">
         <v>0.004271104949584448</v>
@@ -5143,39 +5299,45 @@
         <v>0.004271104949584448</v>
       </c>
       <c r="BG26" t="n">
+        <v>0.004271104949584448</v>
+      </c>
+      <c r="BH26" t="n">
+        <v>0.004271104949584448</v>
+      </c>
+      <c r="BI26" t="n">
         <v>0.004271104949584448</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>83</v>
-      </c>
-      <c r="B27" t="s">
-        <v>126</v>
-      </c>
-      <c r="C27" t="n">
+        <v>85</v>
+      </c>
+      <c r="B27" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="C27" t="s">
+        <v>128</v>
+      </c>
+      <c r="D27" t="n">
         <v>8.549573833746521</v>
       </c>
-      <c r="D27" t="n">
+      <c r="E27" t="n">
         <v>7.829767477913058</v>
       </c>
-      <c r="E27" t="n">
+      <c r="F27" t="n">
         <v>9.303375868878561</v>
       </c>
-      <c r="F27" t="n">
+      <c r="G27" t="n">
         <v>1.4185113284437691</v>
       </c>
-      <c r="G27" t="n">
+      <c r="H27" t="n">
         <v>0.8562820608547748</v>
       </c>
-      <c r="H27" t="n">
+      <c r="I27" t="n">
         <v>2.10926225228759</v>
       </c>
-      <c r="I27" t="n">
-        <v>0.001979833364674377</v>
-      </c>
-      <c r="J27" t="n">
-        <v>0.001979833364674377</v>
+      <c r="J27" t="e">
+        <v>#N/A</v>
       </c>
       <c r="K27" t="n">
         <v>0.001979833364674377</v>
@@ -5202,10 +5364,10 @@
         <v>0.001979833364674377</v>
       </c>
       <c r="S27" t="n">
-        <v>0.0019580943640742808</v>
+        <v>0.001979833364674377</v>
       </c>
       <c r="T27" t="n">
-        <v>0.0019580943640742808</v>
+        <v>0.001979833364674377</v>
       </c>
       <c r="U27" t="n">
         <v>0.0019580943640742808</v>
@@ -5232,10 +5394,10 @@
         <v>0.0019580943640742808</v>
       </c>
       <c r="AC27" t="n">
-        <v>0.0019365936307575993</v>
+        <v>0.0019580943640742808</v>
       </c>
       <c r="AD27" t="n">
-        <v>0.0019365936307575993</v>
+        <v>0.0019580943640742808</v>
       </c>
       <c r="AE27" t="n">
         <v>0.0019365936307575993</v>
@@ -5262,10 +5424,10 @@
         <v>0.0019365936307575993</v>
       </c>
       <c r="AM27" t="n">
-        <v>0.0019155110517711017</v>
+        <v>0.0019365936307575993</v>
       </c>
       <c r="AN27" t="n">
-        <v>0.0019155110517711017</v>
+        <v>0.0019365936307575993</v>
       </c>
       <c r="AO27" t="n">
         <v>0.0019155110517711017</v>
@@ -5292,10 +5454,10 @@
         <v>0.0019155110517711017</v>
       </c>
       <c r="AW27" t="n">
-        <v>0.0018948599818597422</v>
+        <v>0.0019155110517711017</v>
       </c>
       <c r="AX27" t="n">
-        <v>0.0018948599818597422</v>
+        <v>0.0019155110517711017</v>
       </c>
       <c r="AY27" t="n">
         <v>0.0018948599818597422</v>
@@ -5322,39 +5484,45 @@
         <v>0.0018948599818597422</v>
       </c>
       <c r="BG27" t="n">
+        <v>0.0018948599818597422</v>
+      </c>
+      <c r="BH27" t="n">
+        <v>0.0018948599818597422</v>
+      </c>
+      <c r="BI27" t="n">
         <v>0.0018948599818597422</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>84</v>
-      </c>
-      <c r="B28" t="s">
-        <v>127</v>
-      </c>
-      <c r="C28" t="n">
+        <v>86</v>
+      </c>
+      <c r="B28" t="n">
+        <v>27.0</v>
+      </c>
+      <c r="C28" t="s">
+        <v>129</v>
+      </c>
+      <c r="D28" t="n">
         <v>13.61099661422013</v>
       </c>
-      <c r="D28" t="n">
+      <c r="E28" t="n">
         <v>12.669736890602351</v>
       </c>
-      <c r="E28" t="n">
+      <c r="F28" t="n">
         <v>14.377465904289108</v>
       </c>
-      <c r="F28" t="n">
+      <c r="G28" t="n">
         <v>1.8540680716992668</v>
       </c>
-      <c r="G28" t="n">
+      <c r="H28" t="n">
         <v>1.4798519303935744</v>
       </c>
-      <c r="H28" t="n">
+      <c r="I28" t="n">
         <v>2.342017155121072</v>
       </c>
-      <c r="I28" t="n">
-        <v>0.010657683619233183</v>
-      </c>
-      <c r="J28" t="n">
-        <v>0.010657683619233183</v>
+      <c r="J28" t="e">
+        <v>#N/A</v>
       </c>
       <c r="K28" t="n">
         <v>0.010657683619233183</v>
@@ -5381,10 +5549,10 @@
         <v>0.010657683619233183</v>
       </c>
       <c r="S28" t="n">
-        <v>0.003344924058753662</v>
+        <v>0.010657683619233183</v>
       </c>
       <c r="T28" t="n">
-        <v>0.003344924058753662</v>
+        <v>0.010657683619233183</v>
       </c>
       <c r="U28" t="n">
         <v>0.003344924058753662</v>
@@ -5411,10 +5579,10 @@
         <v>0.003344924058753662</v>
       </c>
       <c r="AC28" t="n">
-        <v>0.003270282502349886</v>
+        <v>0.003344924058753662</v>
       </c>
       <c r="AD28" t="n">
-        <v>0.003270282502349886</v>
+        <v>0.003344924058753662</v>
       </c>
       <c r="AE28" t="n">
         <v>0.003270282502349886</v>
@@ -5441,10 +5609,10 @@
         <v>0.003270282502349886</v>
       </c>
       <c r="AM28" t="n">
-        <v>0.0032179423681367504</v>
+        <v>0.003270282502349886</v>
       </c>
       <c r="AN28" t="n">
-        <v>0.0032179423681367504</v>
+        <v>0.003270282502349886</v>
       </c>
       <c r="AO28" t="n">
         <v>0.0032179423681367504</v>
@@ -5471,10 +5639,10 @@
         <v>0.0032179423681367504</v>
       </c>
       <c r="AW28" t="n">
-        <v>0.003166441316068891</v>
+        <v>0.0032179423681367504</v>
       </c>
       <c r="AX28" t="n">
-        <v>0.003166441316068891</v>
+        <v>0.0032179423681367504</v>
       </c>
       <c r="AY28" t="n">
         <v>0.003166441316068891</v>
@@ -5501,69 +5669,75 @@
         <v>0.003166441316068891</v>
       </c>
       <c r="BG28" t="n">
+        <v>0.003166441316068891</v>
+      </c>
+      <c r="BH28" t="n">
+        <v>0.003166441316068891</v>
+      </c>
+      <c r="BI28" t="n">
         <v>0.003166441316068891</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>85</v>
-      </c>
-      <c r="B29" t="s">
-        <v>128</v>
-      </c>
-      <c r="C29" t="n">
+        <v>87</v>
+      </c>
+      <c r="B29" t="n">
+        <v>28.0</v>
+      </c>
+      <c r="C29" t="s">
+        <v>130</v>
+      </c>
+      <c r="D29" t="n">
         <v>8.808542131057255</v>
       </c>
-      <c r="D29" t="n">
+      <c r="E29" t="n">
         <v>8.092553356987393</v>
       </c>
-      <c r="E29" t="n">
+      <c r="F29" t="n">
         <v>9.684922620502192</v>
       </c>
-      <c r="F29" t="n">
+      <c r="G29" t="n">
         <v>1.9316285978073506</v>
       </c>
-      <c r="G29" t="n">
+      <c r="H29" t="n">
         <v>1.7381511358865658</v>
       </c>
-      <c r="H29" t="n">
+      <c r="I29" t="n">
         <v>2.1199515725987643</v>
       </c>
-      <c r="I29" t="n">
-        <v>0.011584879111722656</v>
-      </c>
-      <c r="J29" t="n">
-        <v>0.011584879111722656</v>
+      <c r="J29" t="e">
+        <v>#N/A</v>
       </c>
       <c r="K29" t="n">
-        <v>0.011584879111722656</v>
+        <v>0.011584879111722835</v>
       </c>
       <c r="L29" t="n">
-        <v>0.011584879111722656</v>
+        <v>0.011584879111722835</v>
       </c>
       <c r="M29" t="n">
-        <v>0.011584879111722656</v>
+        <v>0.011584879111722835</v>
       </c>
       <c r="N29" t="n">
-        <v>0.011584879111722656</v>
+        <v>0.011584879111722835</v>
       </c>
       <c r="O29" t="n">
-        <v>0.011584879111722656</v>
+        <v>0.011584879111722835</v>
       </c>
       <c r="P29" t="n">
-        <v>0.011584879111722656</v>
+        <v>0.011584879111722835</v>
       </c>
       <c r="Q29" t="n">
-        <v>0.011584879111722656</v>
+        <v>0.011584879111722835</v>
       </c>
       <c r="R29" t="n">
-        <v>0.011584879111722656</v>
+        <v>0.011584879111722835</v>
       </c>
       <c r="S29" t="n">
-        <v>0.008713165629772136</v>
+        <v>0.011584879111722835</v>
       </c>
       <c r="T29" t="n">
-        <v>0.008713165629772136</v>
+        <v>0.011584879111722835</v>
       </c>
       <c r="U29" t="n">
         <v>0.008713165629772136</v>
@@ -5590,10 +5764,10 @@
         <v>0.008713165629772136</v>
       </c>
       <c r="AC29" t="n">
-        <v>0.005053796237126207</v>
+        <v>0.008713165629772136</v>
       </c>
       <c r="AD29" t="n">
-        <v>0.005053796237126207</v>
+        <v>0.008713165629772136</v>
       </c>
       <c r="AE29" t="n">
         <v>0.005053796237126207</v>
@@ -5620,10 +5794,10 @@
         <v>0.005053796237126207</v>
       </c>
       <c r="AM29" t="n">
-        <v>0.004911021424427809</v>
+        <v>0.005053796237126207</v>
       </c>
       <c r="AN29" t="n">
-        <v>0.004911021424427809</v>
+        <v>0.005053796237126207</v>
       </c>
       <c r="AO29" t="n">
         <v>0.004911021424427809</v>
@@ -5650,10 +5824,10 @@
         <v>0.004911021424427809</v>
       </c>
       <c r="AW29" t="n">
-        <v>0.00478037829868132</v>
+        <v>0.004911021424427809</v>
       </c>
       <c r="AX29" t="n">
-        <v>0.00478037829868132</v>
+        <v>0.004911021424427809</v>
       </c>
       <c r="AY29" t="n">
         <v>0.00478037829868132</v>
@@ -5680,39 +5854,45 @@
         <v>0.00478037829868132</v>
       </c>
       <c r="BG29" t="n">
+        <v>0.00478037829868132</v>
+      </c>
+      <c r="BH29" t="n">
+        <v>0.00478037829868132</v>
+      </c>
+      <c r="BI29" t="n">
         <v>0.00478037829868132</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>86</v>
-      </c>
-      <c r="B30" t="s">
-        <v>129</v>
-      </c>
-      <c r="C30" t="n">
+        <v>88</v>
+      </c>
+      <c r="B30" t="n">
+        <v>29.0</v>
+      </c>
+      <c r="C30" t="s">
+        <v>131</v>
+      </c>
+      <c r="D30" t="n">
         <v>5.0350037596177835</v>
       </c>
-      <c r="D30" t="n">
+      <c r="E30" t="n">
         <v>4.0701689967176975</v>
       </c>
-      <c r="E30" t="n">
+      <c r="F30" t="n">
         <v>6.14617594017135</v>
       </c>
-      <c r="F30" t="n">
+      <c r="G30" t="n">
         <v>1.2837387073917896</v>
       </c>
-      <c r="G30" t="n">
+      <c r="H30" t="n">
         <v>0.9077698877928781</v>
       </c>
-      <c r="H30" t="n">
+      <c r="I30" t="n">
         <v>1.7309314506689193</v>
       </c>
-      <c r="I30" t="n">
-        <v>0.009051437905748295</v>
-      </c>
-      <c r="J30" t="n">
-        <v>0.009051437905748295</v>
+      <c r="J30" t="e">
+        <v>#N/A</v>
       </c>
       <c r="K30" t="n">
         <v>0.009051437905748295</v>
@@ -5739,10 +5919,10 @@
         <v>0.009051437905748295</v>
       </c>
       <c r="S30" t="n">
-        <v>0.0047158979978266565</v>
+        <v>0.009051437905748295</v>
       </c>
       <c r="T30" t="n">
-        <v>0.0047158979978266565</v>
+        <v>0.009051437905748295</v>
       </c>
       <c r="U30" t="n">
         <v>0.0047158979978266565</v>
@@ -5769,10 +5949,10 @@
         <v>0.0047158979978266565</v>
       </c>
       <c r="AC30" t="n">
-        <v>0.004521269724352806</v>
+        <v>0.0047158979978266565</v>
       </c>
       <c r="AD30" t="n">
-        <v>0.004521269724352806</v>
+        <v>0.0047158979978266565</v>
       </c>
       <c r="AE30" t="n">
         <v>0.004521269724352806</v>
@@ -5799,10 +5979,10 @@
         <v>0.004521269724352806</v>
       </c>
       <c r="AM30" t="n">
-        <v>0.004353913599949877</v>
+        <v>0.004521269724352806</v>
       </c>
       <c r="AN30" t="n">
-        <v>0.004353913599949877</v>
+        <v>0.004521269724352806</v>
       </c>
       <c r="AO30" t="n">
         <v>0.004353913599949877</v>
@@ -5829,10 +6009,10 @@
         <v>0.004353913599949877</v>
       </c>
       <c r="AW30" t="n">
-        <v>0.00420376244504479</v>
+        <v>0.004353913599949877</v>
       </c>
       <c r="AX30" t="n">
-        <v>0.00420376244504479</v>
+        <v>0.004353913599949877</v>
       </c>
       <c r="AY30" t="n">
         <v>0.00420376244504479</v>
@@ -5859,39 +6039,45 @@
         <v>0.00420376244504479</v>
       </c>
       <c r="BG30" t="n">
+        <v>0.00420376244504479</v>
+      </c>
+      <c r="BH30" t="n">
+        <v>0.00420376244504479</v>
+      </c>
+      <c r="BI30" t="n">
         <v>0.00420376244504479</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>87</v>
-      </c>
-      <c r="B31" t="s">
-        <v>130</v>
-      </c>
-      <c r="C31" t="n">
+        <v>89</v>
+      </c>
+      <c r="B31" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="C31" t="s">
+        <v>132</v>
+      </c>
+      <c r="D31" t="n">
         <v>2.2452094097094832</v>
       </c>
-      <c r="D31" t="n">
+      <c r="E31" t="n">
         <v>1.7815267182638865</v>
       </c>
-      <c r="E31" t="n">
+      <c r="F31" t="n">
         <v>2.6321686638161284</v>
       </c>
-      <c r="F31" t="n">
+      <c r="G31" t="n">
         <v>1.1020529361229627</v>
       </c>
-      <c r="G31" t="n">
+      <c r="H31" t="n">
         <v>0.558572022050883</v>
       </c>
-      <c r="H31" t="n">
+      <c r="I31" t="n">
         <v>1.66488574240381</v>
       </c>
-      <c r="I31" t="n">
-        <v>0.010414708885557834</v>
-      </c>
-      <c r="J31" t="n">
-        <v>0.010414708885557834</v>
+      <c r="J31" t="e">
+        <v>#N/A</v>
       </c>
       <c r="K31" t="n">
         <v>0.010414708885557834</v>
@@ -5918,10 +6104,10 @@
         <v>0.010414708885557834</v>
       </c>
       <c r="S31" t="n">
-        <v>0.009385823009735094</v>
+        <v>0.010414708885557834</v>
       </c>
       <c r="T31" t="n">
-        <v>0.009385823009735094</v>
+        <v>0.010414708885557834</v>
       </c>
       <c r="U31" t="n">
         <v>0.009385823009735094</v>
@@ -5948,10 +6134,10 @@
         <v>0.009385823009735094</v>
       </c>
       <c r="AC31" t="n">
-        <v>0.008459228701913856</v>
+        <v>0.009385823009735094</v>
       </c>
       <c r="AD31" t="n">
-        <v>0.008459228701913856</v>
+        <v>0.009385823009735094</v>
       </c>
       <c r="AE31" t="n">
         <v>0.008459228701913856</v>
@@ -5978,10 +6164,10 @@
         <v>0.008459228701913856</v>
       </c>
       <c r="AM31" t="n">
-        <v>0.007659734422128939</v>
+        <v>0.008459228701913856</v>
       </c>
       <c r="AN31" t="n">
-        <v>0.007659734422128939</v>
+        <v>0.008459228701913856</v>
       </c>
       <c r="AO31" t="n">
         <v>0.007659734422128939</v>
@@ -6008,10 +6194,10 @@
         <v>0.007659734422128939</v>
       </c>
       <c r="AW31" t="n">
-        <v>0.006909748649664938</v>
+        <v>0.007659734422128939</v>
       </c>
       <c r="AX31" t="n">
-        <v>0.006909748649664938</v>
+        <v>0.007659734422128939</v>
       </c>
       <c r="AY31" t="n">
         <v>0.006909748649664938</v>
@@ -6038,39 +6224,45 @@
         <v>0.006909748649664938</v>
       </c>
       <c r="BG31" t="n">
+        <v>0.006909748649664938</v>
+      </c>
+      <c r="BH31" t="n">
+        <v>0.006909748649664938</v>
+      </c>
+      <c r="BI31" t="n">
         <v>0.006909748649664938</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>88</v>
-      </c>
-      <c r="B32" t="s">
-        <v>131</v>
-      </c>
-      <c r="C32" t="n">
+        <v>90</v>
+      </c>
+      <c r="B32" t="n">
+        <v>31.0</v>
+      </c>
+      <c r="C32" t="s">
+        <v>133</v>
+      </c>
+      <c r="D32" t="n">
         <v>22.02121719217415</v>
       </c>
-      <c r="D32" t="n">
+      <c r="E32" t="n">
         <v>21.062857265478556</v>
       </c>
-      <c r="E32" t="n">
+      <c r="F32" t="n">
         <v>22.767425097605262</v>
       </c>
-      <c r="F32" t="n">
+      <c r="G32" t="n">
         <v>9.321657263243573</v>
       </c>
-      <c r="G32" t="n">
+      <c r="H32" t="n">
         <v>4.642890508046964</v>
       </c>
-      <c r="H32" t="n">
+      <c r="I32" t="n">
         <v>14.74290312475432</v>
       </c>
-      <c r="I32" t="n">
-        <v>0.013015995399330293</v>
-      </c>
-      <c r="J32" t="n">
-        <v>0.013015995399330293</v>
+      <c r="J32" t="e">
+        <v>#N/A</v>
       </c>
       <c r="K32" t="n">
         <v>0.013015995399330293</v>
@@ -6097,10 +6289,10 @@
         <v>0.013015995399330293</v>
       </c>
       <c r="S32" t="n">
-        <v>0.012862817554940165</v>
+        <v>0.013015995399330293</v>
       </c>
       <c r="T32" t="n">
-        <v>0.012862817554940165</v>
+        <v>0.013015995399330293</v>
       </c>
       <c r="U32" t="n">
         <v>0.012862817554940165</v>
@@ -6127,10 +6319,10 @@
         <v>0.012862817554940165</v>
       </c>
       <c r="AC32" t="n">
-        <v>0.012711232695150976</v>
+        <v>0.012862817554940165</v>
       </c>
       <c r="AD32" t="n">
-        <v>0.012711232695150976</v>
+        <v>0.012862817554940165</v>
       </c>
       <c r="AE32" t="n">
         <v>0.012711232695150976</v>
@@ -6157,10 +6349,10 @@
         <v>0.012711232695150976</v>
       </c>
       <c r="AM32" t="n">
-        <v>0.01256122501786212</v>
+        <v>0.012711232695150976</v>
       </c>
       <c r="AN32" t="n">
-        <v>0.01256122501786212</v>
+        <v>0.012711232695150976</v>
       </c>
       <c r="AO32" t="n">
         <v>0.01256122501786212</v>
@@ -6187,10 +6379,10 @@
         <v>0.01256122501786212</v>
       </c>
       <c r="AW32" t="n">
-        <v>0.012412777638665596</v>
+        <v>0.01256122501786212</v>
       </c>
       <c r="AX32" t="n">
-        <v>0.012412777638665596</v>
+        <v>0.01256122501786212</v>
       </c>
       <c r="AY32" t="n">
         <v>0.012412777638665596</v>
@@ -6217,39 +6409,45 @@
         <v>0.012412777638665596</v>
       </c>
       <c r="BG32" t="n">
+        <v>0.012412777638665596</v>
+      </c>
+      <c r="BH32" t="n">
+        <v>0.012412777638665596</v>
+      </c>
+      <c r="BI32" t="n">
         <v>0.012412777638665596</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>89</v>
-      </c>
-      <c r="B33" t="s">
-        <v>132</v>
-      </c>
-      <c r="C33" t="n">
+        <v>91</v>
+      </c>
+      <c r="B33" t="n">
+        <v>32.0</v>
+      </c>
+      <c r="C33" t="s">
+        <v>134</v>
+      </c>
+      <c r="D33" t="n">
         <v>23.807800544943237</v>
       </c>
-      <c r="D33" t="n">
+      <c r="E33" t="n">
         <v>22.489412499891888</v>
       </c>
-      <c r="E33" t="n">
+      <c r="F33" t="n">
         <v>24.944493936126115</v>
       </c>
-      <c r="F33" t="n">
+      <c r="G33" t="n">
         <v>2.624333336538033</v>
       </c>
-      <c r="G33" t="n">
+      <c r="H33" t="n">
         <v>1.8353033302866613</v>
       </c>
-      <c r="H33" t="n">
+      <c r="I33" t="n">
         <v>3.5113946924864834</v>
       </c>
-      <c r="I33" t="n">
-        <v>0.0032517275098719266</v>
-      </c>
-      <c r="J33" t="n">
-        <v>0.0032517275098719266</v>
+      <c r="J33" t="e">
+        <v>#N/A</v>
       </c>
       <c r="K33" t="n">
         <v>0.0032517275098719266</v>
@@ -6276,10 +6474,10 @@
         <v>0.0032517275098719266</v>
       </c>
       <c r="S33" t="n">
-        <v>0.0032188432480110053</v>
+        <v>0.0032517275098719266</v>
       </c>
       <c r="T33" t="n">
-        <v>0.0032188432480110053</v>
+        <v>0.0032517275098719266</v>
       </c>
       <c r="U33" t="n">
         <v>0.0032188432480110053</v>
@@ -6306,10 +6504,10 @@
         <v>0.0032188432480110053</v>
       </c>
       <c r="AC33" t="n">
-        <v>0.002756245170448146</v>
+        <v>0.0032188432480110053</v>
       </c>
       <c r="AD33" t="n">
-        <v>0.002756245170448146</v>
+        <v>0.0032188432480110053</v>
       </c>
       <c r="AE33" t="n">
         <v>0.002756245170448146</v>
@@ -6336,10 +6534,10 @@
         <v>0.002756245170448146</v>
       </c>
       <c r="AM33" t="n">
-        <v>0.002111676332883583</v>
+        <v>0.002756245170448146</v>
       </c>
       <c r="AN33" t="n">
-        <v>0.002111676332883583</v>
+        <v>0.002756245170448146</v>
       </c>
       <c r="AO33" t="n">
         <v>0.002111676332883583</v>
@@ -6366,10 +6564,10 @@
         <v>0.002111676332883583</v>
       </c>
       <c r="AW33" t="n">
-        <v>0.001914497962977002</v>
+        <v>0.002111676332883583</v>
       </c>
       <c r="AX33" t="n">
-        <v>0.001914497962977002</v>
+        <v>0.002111676332883583</v>
       </c>
       <c r="AY33" t="n">
         <v>0.001914497962977002</v>
@@ -6396,39 +6594,45 @@
         <v>0.001914497962977002</v>
       </c>
       <c r="BG33" t="n">
+        <v>0.001914497962977002</v>
+      </c>
+      <c r="BH33" t="n">
+        <v>0.001914497962977002</v>
+      </c>
+      <c r="BI33" t="n">
         <v>0.001914497962977002</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>90</v>
-      </c>
-      <c r="B34" t="s">
-        <v>133</v>
-      </c>
-      <c r="C34" t="n">
+        <v>92</v>
+      </c>
+      <c r="B34" t="n">
+        <v>33.0</v>
+      </c>
+      <c r="C34" t="s">
+        <v>135</v>
+      </c>
+      <c r="D34" t="n">
         <v>15.27924770137309</v>
       </c>
-      <c r="D34" t="n">
+      <c r="E34" t="n">
         <v>12.603134573795256</v>
       </c>
-      <c r="E34" t="n">
+      <c r="F34" t="n">
         <v>16.889163681713605</v>
       </c>
-      <c r="F34" t="n">
+      <c r="G34" t="n">
         <v>0.7384151496010309</v>
       </c>
-      <c r="G34" t="n">
+      <c r="H34" t="n">
         <v>-0.21388897742040458</v>
       </c>
-      <c r="H34" t="n">
+      <c r="I34" t="n">
         <v>1.4531135781550781</v>
       </c>
-      <c r="I34" t="n">
-        <v>0.004671365319447673</v>
-      </c>
-      <c r="J34" t="n">
-        <v>0.004671365319447673</v>
+      <c r="J34" t="e">
+        <v>#N/A</v>
       </c>
       <c r="K34" t="n">
         <v>0.004671365319447673</v>
@@ -6455,10 +6659,10 @@
         <v>0.004671365319447673</v>
       </c>
       <c r="S34" t="n">
-        <v>0.004597263368468418</v>
+        <v>0.004671365319447673</v>
       </c>
       <c r="T34" t="n">
-        <v>0.004597263368468418</v>
+        <v>0.004671365319447673</v>
       </c>
       <c r="U34" t="n">
         <v>0.004597263368468418</v>
@@ -6485,10 +6689,10 @@
         <v>0.004597263368468418</v>
       </c>
       <c r="AC34" t="n">
-        <v>0.0035598104485513814</v>
+        <v>0.004597263368468418</v>
       </c>
       <c r="AD34" t="n">
-        <v>0.0035598104485513814</v>
+        <v>0.004597263368468418</v>
       </c>
       <c r="AE34" t="n">
         <v>0.0035598104485513814</v>
@@ -6515,10 +6719,10 @@
         <v>0.0035598104485513814</v>
       </c>
       <c r="AM34" t="n">
-        <v>0.0016329604696666777</v>
+        <v>0.0035598104485513814</v>
       </c>
       <c r="AN34" t="n">
-        <v>0.0016329604696666777</v>
+        <v>0.0035598104485513814</v>
       </c>
       <c r="AO34" t="n">
         <v>0.0016329604696666777</v>
@@ -6545,10 +6749,10 @@
         <v>0.0016329604696666777</v>
       </c>
       <c r="AW34" t="n">
-        <v>9.201598506448861E-4</v>
+        <v>0.0016329604696666777</v>
       </c>
       <c r="AX34" t="n">
-        <v>9.201598506448861E-4</v>
+        <v>0.0016329604696666777</v>
       </c>
       <c r="AY34" t="n">
         <v>9.201598506448861E-4</v>
@@ -6575,39 +6779,45 @@
         <v>9.201598506448861E-4</v>
       </c>
       <c r="BG34" t="n">
+        <v>9.201598506448861E-4</v>
+      </c>
+      <c r="BH34" t="n">
+        <v>9.201598506448861E-4</v>
+      </c>
+      <c r="BI34" t="n">
         <v>9.201598506448861E-4</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>91</v>
-      </c>
-      <c r="B35" t="s">
-        <v>134</v>
-      </c>
-      <c r="C35" t="n">
+        <v>93</v>
+      </c>
+      <c r="B35" t="n">
+        <v>34.0</v>
+      </c>
+      <c r="C35" t="s">
+        <v>136</v>
+      </c>
+      <c r="D35" t="n">
         <v>6.083492104252233</v>
       </c>
-      <c r="D35" t="n">
+      <c r="E35" t="n">
         <v>4.663822828562308</v>
       </c>
-      <c r="E35" t="n">
+      <c r="F35" t="n">
         <v>7.566069953115533</v>
       </c>
-      <c r="F35" t="n">
+      <c r="G35" t="n">
         <v>1.1293771700956627</v>
       </c>
-      <c r="G35" t="n">
+      <c r="H35" t="n">
         <v>0.7530784217478426</v>
       </c>
-      <c r="H35" t="n">
+      <c r="I35" t="n">
         <v>1.5629134485762595</v>
       </c>
-      <c r="I35" t="n">
-        <v>0.011702430096031603</v>
-      </c>
-      <c r="J35" t="n">
-        <v>0.011702430096031603</v>
+      <c r="J35" t="e">
+        <v>#N/A</v>
       </c>
       <c r="K35" t="n">
         <v>0.011702430096031603</v>
@@ -6634,10 +6844,10 @@
         <v>0.011702430096031603</v>
       </c>
       <c r="S35" t="n">
-        <v>0.006302033070511292</v>
+        <v>0.011702430096031603</v>
       </c>
       <c r="T35" t="n">
-        <v>0.006302033070511292</v>
+        <v>0.011702430096031603</v>
       </c>
       <c r="U35" t="n">
         <v>0.006302033070511292</v>
@@ -6664,10 +6874,10 @@
         <v>0.006302033070511292</v>
       </c>
       <c r="AC35" t="n">
-        <v>0.005351589774579546</v>
+        <v>0.006302033070511292</v>
       </c>
       <c r="AD35" t="n">
-        <v>0.005351589774579546</v>
+        <v>0.006302033070511292</v>
       </c>
       <c r="AE35" t="n">
         <v>0.005351589774579546</v>
@@ -6694,10 +6904,10 @@
         <v>0.005351589774579546</v>
       </c>
       <c r="AM35" t="n">
-        <v>0.005052151660719151</v>
+        <v>0.005351589774579546</v>
       </c>
       <c r="AN35" t="n">
-        <v>0.005052151660719151</v>
+        <v>0.005351589774579546</v>
       </c>
       <c r="AO35" t="n">
         <v>0.005052151660719151</v>
@@ -6724,10 +6934,10 @@
         <v>0.005052151660719151</v>
       </c>
       <c r="AW35" t="n">
-        <v>0.004777837522300521</v>
+        <v>0.005052151660719151</v>
       </c>
       <c r="AX35" t="n">
-        <v>0.004777837522300521</v>
+        <v>0.005052151660719151</v>
       </c>
       <c r="AY35" t="n">
         <v>0.004777837522300521</v>
@@ -6754,39 +6964,45 @@
         <v>0.004777837522300521</v>
       </c>
       <c r="BG35" t="n">
+        <v>0.004777837522300521</v>
+      </c>
+      <c r="BH35" t="n">
+        <v>0.004777837522300521</v>
+      </c>
+      <c r="BI35" t="n">
         <v>0.004777837522300521</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>92</v>
-      </c>
-      <c r="B36" t="s">
-        <v>135</v>
-      </c>
-      <c r="C36" t="n">
+        <v>94</v>
+      </c>
+      <c r="B36" t="n">
+        <v>35.0</v>
+      </c>
+      <c r="C36" t="s">
+        <v>137</v>
+      </c>
+      <c r="D36" t="n">
         <v>3.6376586300317912</v>
       </c>
-      <c r="D36" t="n">
+      <c r="E36" t="n">
         <v>2.460324257229527</v>
       </c>
-      <c r="E36" t="n">
+      <c r="F36" t="n">
         <v>5.392220743479413</v>
       </c>
-      <c r="F36" t="n">
+      <c r="G36" t="n">
         <v>1.56983348134091</v>
       </c>
-      <c r="G36" t="n">
+      <c r="H36" t="n">
         <v>0.7525388724201135</v>
       </c>
-      <c r="H36" t="n">
+      <c r="I36" t="n">
         <v>2.2649615878569422</v>
       </c>
-      <c r="I36" t="n">
-        <v>0.026634300964966794</v>
-      </c>
-      <c r="J36" t="n">
-        <v>0.026634300964966794</v>
+      <c r="J36" t="e">
+        <v>#N/A</v>
       </c>
       <c r="K36" t="n">
         <v>0.026634300964966794</v>
@@ -6813,10 +7029,10 @@
         <v>0.026634300964966794</v>
       </c>
       <c r="S36" t="n">
-        <v>0.02341979999873258</v>
+        <v>0.026634300964966794</v>
       </c>
       <c r="T36" t="n">
-        <v>0.02341979999873258</v>
+        <v>0.026634300964966794</v>
       </c>
       <c r="U36" t="n">
         <v>0.02341979999873258</v>
@@ -6843,10 +7059,10 @@
         <v>0.02341979999873258</v>
       </c>
       <c r="AC36" t="n">
-        <v>0.020434970132217067</v>
+        <v>0.02341979999873258</v>
       </c>
       <c r="AD36" t="n">
-        <v>0.020434970132217067</v>
+        <v>0.02341979999873258</v>
       </c>
       <c r="AE36" t="n">
         <v>0.020434970132217067</v>
@@ -6873,10 +7089,10 @@
         <v>0.020434970132217067</v>
       </c>
       <c r="AM36" t="n">
-        <v>0.017992231304806115</v>
+        <v>0.020434970132217067</v>
       </c>
       <c r="AN36" t="n">
-        <v>0.017992231304806115</v>
+        <v>0.020434970132217067</v>
       </c>
       <c r="AO36" t="n">
         <v>0.017992231304806115</v>
@@ -6903,10 +7119,10 @@
         <v>0.017992231304806115</v>
       </c>
       <c r="AW36" t="n">
-        <v>0.016424600556010915</v>
+        <v>0.017992231304806115</v>
       </c>
       <c r="AX36" t="n">
-        <v>0.016424600556010915</v>
+        <v>0.017992231304806115</v>
       </c>
       <c r="AY36" t="n">
         <v>0.016424600556010915</v>
@@ -6933,39 +7149,45 @@
         <v>0.016424600556010915</v>
       </c>
       <c r="BG36" t="n">
+        <v>0.016424600556010915</v>
+      </c>
+      <c r="BH36" t="n">
+        <v>0.016424600556010915</v>
+      </c>
+      <c r="BI36" t="n">
         <v>0.016424600556010915</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>93</v>
-      </c>
-      <c r="B37" t="s">
-        <v>136</v>
-      </c>
-      <c r="C37" t="n">
+        <v>95</v>
+      </c>
+      <c r="B37" t="n">
+        <v>36.0</v>
+      </c>
+      <c r="C37" t="s">
+        <v>138</v>
+      </c>
+      <c r="D37" t="n">
         <v>6.534735277808329</v>
       </c>
-      <c r="D37" t="n">
+      <c r="E37" t="n">
         <v>5.134852709826179</v>
       </c>
-      <c r="E37" t="n">
+      <c r="F37" t="n">
         <v>8.64852432671963</v>
       </c>
-      <c r="F37" t="n">
+      <c r="G37" t="n">
         <v>1.9154557319179004</v>
       </c>
-      <c r="G37" t="n">
+      <c r="H37" t="n">
         <v>0.5306783308003249</v>
       </c>
-      <c r="H37" t="n">
+      <c r="I37" t="n">
         <v>3.264814160275114</v>
       </c>
-      <c r="I37" t="n">
-        <v>0.013288906512341336</v>
-      </c>
-      <c r="J37" t="n">
-        <v>0.013288906512341336</v>
+      <c r="J37" t="e">
+        <v>#N/A</v>
       </c>
       <c r="K37" t="n">
         <v>0.013288906512341336</v>
@@ -6992,10 +7214,10 @@
         <v>0.013288906512341336</v>
       </c>
       <c r="S37" t="n">
-        <v>0.012750646770708451</v>
+        <v>0.013288906512341336</v>
       </c>
       <c r="T37" t="n">
-        <v>0.012750646770708451</v>
+        <v>0.013288906512341336</v>
       </c>
       <c r="U37" t="n">
         <v>0.012750646770708451</v>
@@ -7022,10 +7244,10 @@
         <v>0.012750646770708451</v>
       </c>
       <c r="AC37" t="n">
-        <v>0.012223421570202042</v>
+        <v>0.012750646770708451</v>
       </c>
       <c r="AD37" t="n">
-        <v>0.012223421570202042</v>
+        <v>0.012750646770708451</v>
       </c>
       <c r="AE37" t="n">
         <v>0.012223421570202042</v>
@@ -7052,10 +7274,10 @@
         <v>0.012223421570202042</v>
       </c>
       <c r="AM37" t="n">
-        <v>0.011677925580069104</v>
+        <v>0.012223421570202042</v>
       </c>
       <c r="AN37" t="n">
-        <v>0.011677925580069104</v>
+        <v>0.012223421570202042</v>
       </c>
       <c r="AO37" t="n">
         <v>0.011677925580069104</v>
@@ -7082,10 +7304,10 @@
         <v>0.011677925580069104</v>
       </c>
       <c r="AW37" t="n">
-        <v>0.011804250098567027</v>
+        <v>0.011677925580069104</v>
       </c>
       <c r="AX37" t="n">
-        <v>0.011804250098567027</v>
+        <v>0.011677925580069104</v>
       </c>
       <c r="AY37" t="n">
         <v>0.011804250098567027</v>
@@ -7112,39 +7334,45 @@
         <v>0.011804250098567027</v>
       </c>
       <c r="BG37" t="n">
+        <v>0.011804250098567027</v>
+      </c>
+      <c r="BH37" t="n">
+        <v>0.011804250098567027</v>
+      </c>
+      <c r="BI37" t="n">
         <v>0.011804250098567027</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>94</v>
-      </c>
-      <c r="B38" t="s">
-        <v>137</v>
-      </c>
-      <c r="C38" t="n">
+        <v>96</v>
+      </c>
+      <c r="B38" t="n">
+        <v>37.0</v>
+      </c>
+      <c r="C38" t="s">
+        <v>139</v>
+      </c>
+      <c r="D38" t="n">
         <v>4.8323285642403295</v>
       </c>
-      <c r="D38" t="n">
+      <c r="E38" t="n">
         <v>3.3778509864102704</v>
       </c>
-      <c r="E38" t="n">
+      <c r="F38" t="n">
         <v>7.699723977009755</v>
       </c>
-      <c r="F38" t="n">
+      <c r="G38" t="n">
         <v>1.7603198807253868</v>
       </c>
-      <c r="G38" t="n">
+      <c r="H38" t="n">
         <v>0.9809130537293194</v>
       </c>
-      <c r="H38" t="n">
+      <c r="I38" t="n">
         <v>2.7484991490057604</v>
       </c>
-      <c r="I38" t="n">
-        <v>0.03950581064589507</v>
-      </c>
-      <c r="J38" t="n">
-        <v>0.03950581064589507</v>
+      <c r="J38" t="e">
+        <v>#N/A</v>
       </c>
       <c r="K38" t="n">
         <v>0.03950581064589507</v>
@@ -7171,10 +7399,10 @@
         <v>0.03950581064589507</v>
       </c>
       <c r="S38" t="n">
-        <v>0.03418493141312118</v>
+        <v>0.03950581064589507</v>
       </c>
       <c r="T38" t="n">
-        <v>0.03418493141312118</v>
+        <v>0.03950581064589507</v>
       </c>
       <c r="U38" t="n">
         <v>0.03418493141312118</v>
@@ -7201,10 +7429,10 @@
         <v>0.03418493141312118</v>
       </c>
       <c r="AC38" t="n">
-        <v>0.02995151836360612</v>
+        <v>0.03418493141312118</v>
       </c>
       <c r="AD38" t="n">
-        <v>0.02995151836360612</v>
+        <v>0.03418493141312118</v>
       </c>
       <c r="AE38" t="n">
         <v>0.02995151836360612</v>
@@ -7231,10 +7459,10 @@
         <v>0.02995151836360612</v>
       </c>
       <c r="AM38" t="n">
-        <v>0.0383596216067779</v>
+        <v>0.02995151836360612</v>
       </c>
       <c r="AN38" t="n">
-        <v>0.0383596216067779</v>
+        <v>0.02995151836360612</v>
       </c>
       <c r="AO38" t="n">
         <v>0.0383596216067779</v>
@@ -7261,10 +7489,10 @@
         <v>0.0383596216067779</v>
       </c>
       <c r="AW38" t="n">
-        <v>0.0</v>
+        <v>0.0383596216067779</v>
       </c>
       <c r="AX38" t="n">
-        <v>0.0</v>
+        <v>0.0383596216067779</v>
       </c>
       <c r="AY38" t="n">
         <v>0.0</v>
@@ -7291,39 +7519,45 @@
         <v>0.0</v>
       </c>
       <c r="BG38" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BH38" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BI38" t="n">
         <v>0.0</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>95</v>
-      </c>
-      <c r="B39" t="s">
-        <v>138</v>
-      </c>
-      <c r="C39" t="n">
+        <v>97</v>
+      </c>
+      <c r="B39" t="n">
+        <v>38.0</v>
+      </c>
+      <c r="C39" t="s">
+        <v>140</v>
+      </c>
+      <c r="D39" t="n">
         <v>11.87044024185835</v>
       </c>
-      <c r="D39" t="n">
+      <c r="E39" t="n">
         <v>8.176831946533301</v>
       </c>
-      <c r="E39" t="n">
+      <c r="F39" t="n">
         <v>15.386057843873237</v>
       </c>
-      <c r="F39" t="n">
+      <c r="G39" t="n">
         <v>6.549541015623335</v>
       </c>
-      <c r="G39" t="n">
+      <c r="H39" t="n">
         <v>2.92462731804467</v>
       </c>
-      <c r="H39" t="n">
+      <c r="I39" t="n">
         <v>10.032003326183121</v>
       </c>
-      <c r="I39" t="n">
-        <v>0.023194988844705656</v>
-      </c>
-      <c r="J39" t="n">
-        <v>0.023194988844705656</v>
+      <c r="J39" t="e">
+        <v>#N/A</v>
       </c>
       <c r="K39" t="n">
         <v>0.023194988844705656</v>
@@ -7350,10 +7584,10 @@
         <v>0.023194988844705656</v>
       </c>
       <c r="S39" t="n">
-        <v>0.022398359123774813</v>
+        <v>0.023194988844705656</v>
       </c>
       <c r="T39" t="n">
-        <v>0.022398359123774813</v>
+        <v>0.023194988844705656</v>
       </c>
       <c r="U39" t="n">
         <v>0.022398359123774813</v>
@@ -7380,10 +7614,10 @@
         <v>0.022398359123774813</v>
       </c>
       <c r="AC39" t="n">
-        <v>0.021628103589952728</v>
+        <v>0.022398359123774813</v>
       </c>
       <c r="AD39" t="n">
-        <v>0.021628103589952728</v>
+        <v>0.022398359123774813</v>
       </c>
       <c r="AE39" t="n">
         <v>0.021628103589952728</v>
@@ -7410,10 +7644,10 @@
         <v>0.021628103589952728</v>
       </c>
       <c r="AM39" t="n">
-        <v>0.02088336112896707</v>
+        <v>0.021628103589952728</v>
       </c>
       <c r="AN39" t="n">
-        <v>0.02088336112896707</v>
+        <v>0.021628103589952728</v>
       </c>
       <c r="AO39" t="n">
         <v>0.02088336112896707</v>
@@ -7440,10 +7674,10 @@
         <v>0.02088336112896707</v>
       </c>
       <c r="AW39" t="n">
-        <v>0.02016332375161527</v>
+        <v>0.02088336112896707</v>
       </c>
       <c r="AX39" t="n">
-        <v>0.02016332375161527</v>
+        <v>0.02088336112896707</v>
       </c>
       <c r="AY39" t="n">
         <v>0.02016332375161527</v>
@@ -7470,39 +7704,45 @@
         <v>0.02016332375161527</v>
       </c>
       <c r="BG39" t="n">
+        <v>0.02016332375161527</v>
+      </c>
+      <c r="BH39" t="n">
+        <v>0.02016332375161527</v>
+      </c>
+      <c r="BI39" t="n">
         <v>0.02016332375161527</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>96</v>
-      </c>
-      <c r="B40" t="s">
-        <v>139</v>
-      </c>
-      <c r="C40" t="n">
+        <v>98</v>
+      </c>
+      <c r="B40" t="n">
+        <v>39.0</v>
+      </c>
+      <c r="C40" t="s">
+        <v>141</v>
+      </c>
+      <c r="D40" t="n">
         <v>2.761458118238965</v>
       </c>
-      <c r="D40" t="n">
+      <c r="E40" t="n">
         <v>1.7801766239479162</v>
       </c>
-      <c r="E40" t="n">
+      <c r="F40" t="n">
         <v>4.337420912902429</v>
       </c>
-      <c r="F40" t="n">
+      <c r="G40" t="n">
         <v>0.48007949889323875</v>
       </c>
-      <c r="G40" t="n">
+      <c r="H40" t="n">
         <v>0.3139357116804067</v>
       </c>
-      <c r="H40" t="n">
+      <c r="I40" t="n">
         <v>0.8327972847894829</v>
       </c>
-      <c r="I40" t="n">
-        <v>0.021247761094455152</v>
-      </c>
-      <c r="J40" t="n">
-        <v>0.021247761094455152</v>
+      <c r="J40" t="e">
+        <v>#N/A</v>
       </c>
       <c r="K40" t="n">
         <v>0.021247761094455152</v>
@@ -7529,10 +7769,10 @@
         <v>0.021247761094455152</v>
       </c>
       <c r="S40" t="n">
-        <v>0.0031372594183209255</v>
+        <v>0.021247761094455152</v>
       </c>
       <c r="T40" t="n">
-        <v>0.0031372594183209255</v>
+        <v>0.021247761094455152</v>
       </c>
       <c r="U40" t="n">
         <v>0.0031372594183209255</v>
@@ -7559,10 +7799,10 @@
         <v>0.0031372594183209255</v>
       </c>
       <c r="AC40" t="n">
-        <v>0.002242138021867457</v>
+        <v>0.0031372594183209255</v>
       </c>
       <c r="AD40" t="n">
-        <v>0.002242138021867457</v>
+        <v>0.0031372594183209255</v>
       </c>
       <c r="AE40" t="n">
         <v>0.002242138021867457</v>
@@ -7589,10 +7829,10 @@
         <v>0.002242138021867457</v>
       </c>
       <c r="AM40" t="n">
-        <v>0.0020210128031031838</v>
+        <v>0.002242138021867457</v>
       </c>
       <c r="AN40" t="n">
-        <v>0.0020210128031031838</v>
+        <v>0.002242138021867457</v>
       </c>
       <c r="AO40" t="n">
         <v>0.0020210128031031838</v>
@@ -7619,10 +7859,10 @@
         <v>0.0020210128031031838</v>
       </c>
       <c r="AW40" t="n">
-        <v>0.0018164856813673413</v>
+        <v>0.0020210128031031838</v>
       </c>
       <c r="AX40" t="n">
-        <v>0.0018164856813673413</v>
+        <v>0.0020210128031031838</v>
       </c>
       <c r="AY40" t="n">
         <v>0.0018164856813673413</v>
@@ -7649,39 +7889,45 @@
         <v>0.0018164856813673413</v>
       </c>
       <c r="BG40" t="n">
+        <v>0.0018164856813673413</v>
+      </c>
+      <c r="BH40" t="n">
+        <v>0.0018164856813673413</v>
+      </c>
+      <c r="BI40" t="n">
         <v>0.0018164856813673413</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>97</v>
-      </c>
-      <c r="B41" t="s">
-        <v>140</v>
-      </c>
-      <c r="C41" t="n">
+        <v>99</v>
+      </c>
+      <c r="B41" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="C41" t="s">
+        <v>142</v>
+      </c>
+      <c r="D41" t="n">
         <v>14.092440672944168</v>
       </c>
-      <c r="D41" t="n">
+      <c r="E41" t="n">
         <v>11.761868187446836</v>
       </c>
-      <c r="E41" t="n">
+      <c r="F41" t="n">
         <v>17.120275108656955</v>
       </c>
-      <c r="F41" t="n">
+      <c r="G41" t="n">
         <v>4.444658154177577</v>
       </c>
-      <c r="G41" t="n">
+      <c r="H41" t="n">
         <v>3.669594374941772</v>
       </c>
-      <c r="H41" t="n">
+      <c r="I41" t="n">
         <v>5.467724985817945</v>
       </c>
-      <c r="I41" t="n">
-        <v>0.01887879928903864</v>
-      </c>
-      <c r="J41" t="n">
-        <v>0.01887879928903864</v>
+      <c r="J41" t="e">
+        <v>#N/A</v>
       </c>
       <c r="K41" t="n">
         <v>0.01887879928903864</v>
@@ -7708,10 +7954,10 @@
         <v>0.01887879928903864</v>
       </c>
       <c r="S41" t="n">
-        <v>0.018407018088173112</v>
+        <v>0.01887879928903864</v>
       </c>
       <c r="T41" t="n">
-        <v>0.018407018088173112</v>
+        <v>0.01887879928903864</v>
       </c>
       <c r="U41" t="n">
         <v>0.018407018088173112</v>
@@ -7738,10 +7984,10 @@
         <v>0.018407018088173112</v>
       </c>
       <c r="AC41" t="n">
-        <v>0.017945067120237114</v>
+        <v>0.018407018088173112</v>
       </c>
       <c r="AD41" t="n">
-        <v>0.017945067120237114</v>
+        <v>0.018407018088173112</v>
       </c>
       <c r="AE41" t="n">
         <v>0.017945067120237114</v>
@@ -7768,10 +8014,10 @@
         <v>0.017945067120237114</v>
       </c>
       <c r="AM41" t="n">
-        <v>0.017492756960203516</v>
+        <v>0.017945067120237114</v>
       </c>
       <c r="AN41" t="n">
-        <v>0.017492756960203516</v>
+        <v>0.017945067120237114</v>
       </c>
       <c r="AO41" t="n">
         <v>0.017492756960203516</v>
@@ -7798,10 +8044,10 @@
         <v>0.017492756960203516</v>
       </c>
       <c r="AW41" t="n">
-        <v>0.017049917131967973</v>
+        <v>0.017492756960203516</v>
       </c>
       <c r="AX41" t="n">
-        <v>0.017049917131967973</v>
+        <v>0.017492756960203516</v>
       </c>
       <c r="AY41" t="n">
         <v>0.017049917131967973</v>
@@ -7828,39 +8074,45 @@
         <v>0.017049917131967973</v>
       </c>
       <c r="BG41" t="n">
+        <v>0.017049917131967973</v>
+      </c>
+      <c r="BH41" t="n">
+        <v>0.017049917131967973</v>
+      </c>
+      <c r="BI41" t="n">
         <v>0.017049917131967973</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>98</v>
-      </c>
-      <c r="B42" t="s">
-        <v>141</v>
-      </c>
-      <c r="C42" t="n">
+        <v>100</v>
+      </c>
+      <c r="B42" t="n">
+        <v>41.0</v>
+      </c>
+      <c r="C42" t="s">
+        <v>143</v>
+      </c>
+      <c r="D42" t="n">
         <v>8.957289161684976</v>
       </c>
-      <c r="D42" t="n">
+      <c r="E42" t="n">
         <v>7.771644568938647</v>
       </c>
-      <c r="E42" t="n">
+      <c r="F42" t="n">
         <v>10.422901017616526</v>
       </c>
-      <c r="F42" t="n">
+      <c r="G42" t="n">
         <v>4.473941854962428</v>
       </c>
-      <c r="G42" t="n">
+      <c r="H42" t="n">
         <v>3.6486691709315773</v>
       </c>
-      <c r="H42" t="n">
+      <c r="I42" t="n">
         <v>5.463613062753907</v>
       </c>
-      <c r="I42" t="n">
-        <v>0.031220069390474503</v>
-      </c>
-      <c r="J42" t="n">
-        <v>0.031220069390474503</v>
+      <c r="J42" t="e">
+        <v>#N/A</v>
       </c>
       <c r="K42" t="n">
         <v>0.031220069390474503</v>
@@ -7887,10 +8139,10 @@
         <v>0.031220069390474503</v>
       </c>
       <c r="S42" t="n">
-        <v>0.029439849911468575</v>
+        <v>0.031220069390474503</v>
       </c>
       <c r="T42" t="n">
-        <v>0.029439849911468575</v>
+        <v>0.031220069390474503</v>
       </c>
       <c r="U42" t="n">
         <v>0.029439849911468575</v>
@@ -7917,10 +8169,10 @@
         <v>0.029439849911468575</v>
       </c>
       <c r="AC42" t="n">
-        <v>0.027752258041566648</v>
+        <v>0.029439849911468575</v>
       </c>
       <c r="AD42" t="n">
-        <v>0.027752258041566648</v>
+        <v>0.029439849911468575</v>
       </c>
       <c r="AE42" t="n">
         <v>0.027752258041566648</v>
@@ -7947,10 +8199,10 @@
         <v>0.027752258041566648</v>
       </c>
       <c r="AM42" t="n">
-        <v>0.02623893138077702</v>
+        <v>0.027752258041566648</v>
       </c>
       <c r="AN42" t="n">
-        <v>0.02623893138077702</v>
+        <v>0.027752258041566648</v>
       </c>
       <c r="AO42" t="n">
         <v>0.02623893138077702</v>
@@ -7977,10 +8229,10 @@
         <v>0.02623893138077702</v>
       </c>
       <c r="AW42" t="n">
-        <v>0.02477299381169522</v>
+        <v>0.02623893138077702</v>
       </c>
       <c r="AX42" t="n">
-        <v>0.02477299381169522</v>
+        <v>0.02623893138077702</v>
       </c>
       <c r="AY42" t="n">
         <v>0.02477299381169522</v>
@@ -8007,39 +8259,45 @@
         <v>0.02477299381169522</v>
       </c>
       <c r="BG42" t="n">
+        <v>0.02477299381169522</v>
+      </c>
+      <c r="BH42" t="n">
+        <v>0.02477299381169522</v>
+      </c>
+      <c r="BI42" t="n">
         <v>0.02477299381169522</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>99</v>
-      </c>
-      <c r="B43" t="s">
-        <v>142</v>
-      </c>
-      <c r="C43" t="n">
+        <v>101</v>
+      </c>
+      <c r="B43" t="n">
+        <v>42.0</v>
+      </c>
+      <c r="C43" t="s">
+        <v>144</v>
+      </c>
+      <c r="D43" t="n">
         <v>1.931037716992491</v>
       </c>
-      <c r="D43" t="n">
+      <c r="E43" t="n">
         <v>1.4277105978680238</v>
       </c>
-      <c r="E43" t="n">
+      <c r="F43" t="n">
         <v>2.9934685195364574</v>
       </c>
-      <c r="F43" t="n">
+      <c r="G43" t="n">
         <v>0.6013810082764538</v>
       </c>
-      <c r="G43" t="n">
+      <c r="H43" t="n">
         <v>0.3086348830402017</v>
       </c>
-      <c r="H43" t="n">
+      <c r="I43" t="n">
         <v>1.058112549457722</v>
       </c>
-      <c r="I43" t="n">
-        <v>0.06013810082764538</v>
-      </c>
-      <c r="J43" t="n">
-        <v>0.06013810082764538</v>
+      <c r="J43" t="e">
+        <v>#N/A</v>
       </c>
       <c r="K43" t="n">
         <v>0.06013810082764538</v>
@@ -8066,10 +8324,10 @@
         <v>0.06013810082764538</v>
       </c>
       <c r="S43" t="n">
-        <v>0.0</v>
+        <v>0.06013810082764538</v>
       </c>
       <c r="T43" t="n">
-        <v>0.0</v>
+        <v>0.06013810082764538</v>
       </c>
       <c r="U43" t="n">
         <v>0.0</v>
@@ -8186,39 +8444,45 @@
         <v>0.0</v>
       </c>
       <c r="BG43" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BH43" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BI43" t="n">
         <v>0.0</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>100</v>
-      </c>
-      <c r="B44" t="s">
-        <v>143</v>
-      </c>
-      <c r="C44" t="n">
+        <v>102</v>
+      </c>
+      <c r="B44" t="n">
+        <v>43.0</v>
+      </c>
+      <c r="C44" t="s">
+        <v>145</v>
+      </c>
+      <c r="D44" t="n">
         <v>6.446087488169069</v>
       </c>
-      <c r="D44" t="n">
+      <c r="E44" t="n">
         <v>3.549870972763299</v>
       </c>
-      <c r="E44" t="n">
+      <c r="F44" t="n">
         <v>9.387898518200972</v>
       </c>
-      <c r="F44" t="n">
+      <c r="G44" t="n">
         <v>2.709157103993042</v>
       </c>
-      <c r="G44" t="n">
+      <c r="H44" t="n">
         <v>1.4817056248005422</v>
       </c>
-      <c r="H44" t="n">
+      <c r="I44" t="n">
         <v>4.155928153446203</v>
       </c>
-      <c r="I44" t="n">
-        <v>0.27065588107179483</v>
-      </c>
-      <c r="J44" t="n">
-        <v>0.27065588107179483</v>
+      <c r="J44" t="e">
+        <v>#N/A</v>
       </c>
       <c r="K44" t="n">
         <v>0.27065588107179483</v>
@@ -8245,10 +8509,10 @@
         <v>0.27065588107179483</v>
       </c>
       <c r="S44" t="n">
-        <v>9.495948163573686E-6</v>
+        <v>0.27065588107179483</v>
       </c>
       <c r="T44" t="n">
-        <v>9.495948163573686E-6</v>
+        <v>0.27065588107179483</v>
       </c>
       <c r="U44" t="n">
         <v>9.495948163573686E-6</v>
@@ -8275,10 +8539,10 @@
         <v>9.495948163573686E-6</v>
       </c>
       <c r="AC44" t="n">
-        <v>9.130436493065553E-6</v>
+        <v>9.495948163573686E-6</v>
       </c>
       <c r="AD44" t="n">
-        <v>9.130436493065553E-6</v>
+        <v>9.495948163573686E-6</v>
       </c>
       <c r="AE44" t="n">
         <v>9.130436493065553E-6</v>
@@ -8305,10 +8569,10 @@
         <v>9.130436493065553E-6</v>
       </c>
       <c r="AM44" t="n">
-        <v>8.777849842700469E-6</v>
+        <v>9.130436493065553E-6</v>
       </c>
       <c r="AN44" t="n">
-        <v>8.777849842700469E-6</v>
+        <v>9.130436493065553E-6</v>
       </c>
       <c r="AO44" t="n">
         <v>8.777849842700469E-6</v>
@@ -8335,10 +8599,10 @@
         <v>8.777849842700469E-6</v>
       </c>
       <c r="AW44" t="n">
-        <v>8.437794181004321E-6</v>
+        <v>8.777849842700469E-6</v>
       </c>
       <c r="AX44" t="n">
-        <v>8.437794181004321E-6</v>
+        <v>8.777849842700469E-6</v>
       </c>
       <c r="AY44" t="n">
         <v>8.437794181004321E-6</v>
@@ -8365,6 +8629,12 @@
         <v>8.437794181004321E-6</v>
       </c>
       <c r="BG44" t="n">
+        <v>8.437794181004321E-6</v>
+      </c>
+      <c r="BH44" t="n">
+        <v>8.437794181004321E-6</v>
+      </c>
+      <c r="BI44" t="n">
         <v>8.437794181004321E-6</v>
       </c>
     </row>

</xml_diff>